<commit_message>
Change fonts and colours
</commit_message>
<xml_diff>
--- a/OAS 2025.xlsx
+++ b/OAS 2025.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A4C7B9C-1615-4DDC-AFA4-2F3F365D079F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761EEB39-B3E2-4E9C-9258-1F7F4B3EAC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="6" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" firstSheet="8" activeTab="11" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -29,14 +29,14 @@
     <sheet name="Lists" sheetId="9" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current account'!$A$1:$I$354</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current account'!$A$1:$I$353</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Membership List'!$A$2:$A$216</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Stripe!$A$1:$W$478</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId15"/>
-    <pivotCache cacheId="15" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3953" uniqueCount="1577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3982" uniqueCount="1587">
   <si>
     <t>Subs</t>
   </si>
@@ -4789,6 +4789,36 @@
   </si>
   <si>
     <t>SumUp Payments AccMDD PID1044627</t>
+  </si>
+  <si>
+    <t>CASH IN AT 403534</t>
+  </si>
+  <si>
+    <t>WILLIAM HOGG williamHogg</t>
+  </si>
+  <si>
+    <t>A Hermon Tara Palmer Woolwy</t>
+  </si>
+  <si>
+    <t>Caroline Ritson</t>
+  </si>
+  <si>
+    <t>Jill Colchester</t>
+  </si>
+  <si>
+    <t>Hannah Vickery</t>
+  </si>
+  <si>
+    <t>Helan Pakeman</t>
+  </si>
+  <si>
+    <t>SORENSEN BH HELEN PAKEMAN</t>
+  </si>
+  <si>
+    <t>LISTER J&amp;G Jenny Lister</t>
+  </si>
+  <si>
+    <t>Lister</t>
   </si>
 </sst>
 </file>
@@ -4947,7 +4977,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -4990,7 +5020,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyBorder="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5014,13 +5043,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45742.416263888888" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="268" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45744.730815972223" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="274" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I401" sheet="Current account"/>
+    <worksheetSource ref="A1:I400" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-03-26T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-03-29T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5035,7 +5064,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="14064.550000000008"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="15657.970000000008"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
       <sharedItems containsBlank="1" count="19">
@@ -5076,13 +5105,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45742.416487731483" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="268" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45744.730861805554" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="274" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="A1:I504" sheet="Current account"/>
+    <worksheetSource ref="A1:I503" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-03-26T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-03-29T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5097,7 +5126,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="14064.550000000008"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="15657.970000000008"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
       <sharedItems containsBlank="1" count="29">
@@ -5152,7 +5181,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="268">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="274">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -8091,6 +8120,72 @@
     <m/>
   </r>
   <r>
+    <d v="2025-03-26T00:00:00"/>
+    <s v="CR"/>
+    <s v="WILLIAM HOGG williamHogg"/>
+    <m/>
+    <n v="719"/>
+    <n v="14783.550000000008"/>
+    <x v="18"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-26T00:00:00"/>
+    <s v="CR"/>
+    <s v="CASH IN AT 403534"/>
+    <m/>
+    <n v="80.599999999999994"/>
+    <n v="14864.150000000009"/>
+    <x v="15"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-27T00:00:00"/>
+    <s v="CR"/>
+    <s v="A Hermon Tara Palmer Woolwy"/>
+    <m/>
+    <n v="700"/>
+    <n v="15564.150000000009"/>
+    <x v="18"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="BP"/>
+    <s v="Sarah Dearling OAS"/>
+    <n v="15.59"/>
+    <m/>
+    <n v="15548.560000000009"/>
+    <x v="11"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="BP"/>
+    <s v="Sarah Dearling OAS"/>
+    <n v="15.59"/>
+    <m/>
+    <n v="15532.970000000008"/>
+    <x v="11"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="CR"/>
+    <s v="SORENSEN BH HELEN PAKEMAN"/>
+    <m/>
+    <n v="125"/>
+    <n v="15657.970000000008"/>
+    <x v="18"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -8105,7 +8200,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="268">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="274">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -11044,6 +11139,72 @@
     <m/>
   </r>
   <r>
+    <d v="2025-03-26T00:00:00"/>
+    <s v="CR"/>
+    <s v="WILLIAM HOGG williamHogg"/>
+    <m/>
+    <n v="719"/>
+    <n v="14783.550000000008"/>
+    <x v="18"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-26T00:00:00"/>
+    <s v="CR"/>
+    <s v="CASH IN AT 403534"/>
+    <m/>
+    <n v="80.599999999999994"/>
+    <n v="14864.150000000009"/>
+    <x v="15"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-27T00:00:00"/>
+    <s v="CR"/>
+    <s v="A Hermon Tara Palmer Woolwy"/>
+    <m/>
+    <n v="700"/>
+    <n v="15564.150000000009"/>
+    <x v="18"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="BP"/>
+    <s v="Sarah Dearling OAS"/>
+    <n v="15.59"/>
+    <m/>
+    <n v="15548.560000000009"/>
+    <x v="11"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="BP"/>
+    <s v="Sarah Dearling OAS"/>
+    <n v="15.59"/>
+    <m/>
+    <n v="15532.970000000008"/>
+    <x v="11"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-03-28T00:00:00"/>
+    <s v="CR"/>
+    <s v="SORENSEN BH HELEN PAKEMAN"/>
+    <m/>
+    <n v="125"/>
+    <n v="15657.970000000008"/>
+    <x v="18"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -11058,7 +11219,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB64E1A4-8455-499E-80FF-BC0BFCCF7279}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB64E1A4-8455-499E-80FF-BC0BFCCF7279}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C23" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -11187,7 +11348,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -11300,7 +11461,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A19:C34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -11841,7 +12002,7 @@
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="31">
-        <f>SUMIF('Current account'!G2:G402, "Subs", 'Current account'!E2:E402)</f>
+        <f>SUMIF('Current account'!G2:G401, "Subs", 'Current account'!E2:E401)</f>
         <v>0</v>
       </c>
       <c r="L4" s="17"/>
@@ -11850,7 +12011,7 @@
       </c>
       <c r="N4" s="17"/>
       <c r="O4" s="31">
-        <f>SUMIF('Current account'!G2:G402,"Prof Fees",'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401,"Prof Fees",'Current account'!D2:D401)</f>
         <v>0</v>
       </c>
     </row>
@@ -11880,8 +12041,8 @@
       </c>
       <c r="J5" s="17"/>
       <c r="K5" s="31">
-        <f>SUMIF('Current account'!G2:G402, "Subs 2025", 'Current account'!E2:E402)</f>
-        <v>6588.8800000000019</v>
+        <f>SUMIF('Current account'!G2:G401, "Subs 2025", 'Current account'!E2:E401)</f>
+        <v>6618.8800000000019</v>
       </c>
       <c r="L5" s="17"/>
       <c r="M5" s="17" t="s">
@@ -11889,7 +12050,7 @@
       </c>
       <c r="N5" s="17"/>
       <c r="O5" s="31">
-        <f>SUMIF('Current account'!G2:G402,"AGM",'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401,"AGM",'Current account'!D2:D401)</f>
         <v>132</v>
       </c>
     </row>
@@ -11917,7 +12078,7 @@
       </c>
       <c r="J6" s="17"/>
       <c r="K6" s="31">
-        <f>SUMIF('Current account'!G2:G402, "Other income", 'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401, "Other income", 'Current account'!D2:D401)</f>
         <v>0</v>
       </c>
       <c r="L6" s="17"/>
@@ -11926,7 +12087,7 @@
       </c>
       <c r="N6" s="17"/>
       <c r="O6" s="31">
-        <f>SUMIF('Current account'!G2:G402,"Gifts",'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401,"Gifts",'Current account'!D2:D401)</f>
         <v>55.89</v>
       </c>
     </row>
@@ -11961,7 +12122,7 @@
       </c>
       <c r="N7" s="17"/>
       <c r="O7" s="31">
-        <f>SUMIF('Current account'!G2:G402,"Admin",'Current account'!D2:D402)+SUMIF('Current account'!G2:G402, "Other expenses", 'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401,"Admin",'Current account'!D2:D401)+SUMIF('Current account'!G2:G401, "Other expenses", 'Current account'!D2:D401)</f>
         <v>97.6</v>
       </c>
     </row>
@@ -11986,8 +12147,8 @@
       </c>
       <c r="N8" s="17"/>
       <c r="O8" s="31">
-        <f ca="1">SUMIF('Current account'!G2:G402,"Website",'Current account'!D2:D41)</f>
-        <v>7.95</v>
+        <f ca="1">SUMIF('Current account'!G2:G401,"Website",'Current account'!D2:D41)</f>
+        <v>39.129999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -11997,7 +12158,7 @@
       <c r="B9" s="16"/>
       <c r="C9" s="31">
         <f>GETPIVOTDATA("Sum of Income",Exhibitions!$A$3,"Category","Bar sales")</f>
-        <v>159.37</v>
+        <v>239.97</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17" t="s">
@@ -12018,7 +12179,7 @@
       </c>
       <c r="N9" s="17"/>
       <c r="O9" s="31">
-        <f>SUMIF('Current account'!G2:G402, "Insurance", 'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401, "Insurance", 'Current account'!D2:D401)</f>
         <v>613.22</v>
       </c>
     </row>
@@ -12050,7 +12211,7 @@
       </c>
       <c r="N10" s="17"/>
       <c r="O10" s="31">
-        <f>SUMIF('Current account'!G2:G402, "Donations db", 'Current account'!D2:D402)</f>
+        <f>SUMIF('Current account'!G2:G401, "Donations db", 'Current account'!D2:D401)</f>
         <v>200</v>
       </c>
     </row>
@@ -12174,7 +12335,7 @@
       <c r="N15" s="17"/>
       <c r="O15" s="31">
         <f ca="1">SUM(O4:O13)</f>
-        <v>1106.6600000000001</v>
+        <v>1137.8400000000001</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -12367,7 +12528,7 @@
       </c>
       <c r="N23" s="17"/>
       <c r="O23" s="31">
-        <f>'Savings account'!F15+'Current account'!F402</f>
+        <f>'Savings account'!F15+'Current account'!F401</f>
         <v>0</v>
       </c>
     </row>
@@ -12560,8 +12721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABEE55E-E7BE-4AC9-B510-B295735902B8}">
   <dimension ref="A1:U108"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R54" sqref="R2:R54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -25782,15 +25943,16 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3021DE-183F-467F-BF7A-5FF49A8AB64C}">
-  <dimension ref="A1:Z31"/>
+  <dimension ref="A1:Z30"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9" style="5"/>
+    <col min="1" max="1" width="16.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" style="5"/>
     <col min="3" max="3" width="10.08984375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="5"/>
@@ -25844,7 +26006,7 @@
       <c r="S2" s="9"/>
       <c r="U2" s="11"/>
       <c r="Z2" s="20" t="e">
-        <f t="shared" ref="Z2:Z23" si="0">S2/G2</f>
+        <f t="shared" ref="Z2:Z22" si="0">S2/G2</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -25856,11 +26018,11 @@
         <v>240</v>
       </c>
       <c r="D3" s="27">
-        <f t="shared" ref="D3:D8" si="1">0.25 * C3</f>
+        <f t="shared" ref="D3:D16" si="1">0.25 * C3</f>
         <v>60</v>
       </c>
       <c r="E3" s="27">
-        <f t="shared" ref="E3:E8" si="2">C3-D3</f>
+        <f t="shared" ref="E3:E16" si="2">C3-D3</f>
         <v>180</v>
       </c>
       <c r="F3"/>
@@ -25871,7 +26033,7 @@
       <c r="S3" s="9"/>
       <c r="U3" s="10"/>
       <c r="X3" s="12">
-        <f>Q3-N21</f>
+        <f>Q3-N20</f>
         <v>0</v>
       </c>
       <c r="Z3" s="20" t="e">
@@ -26007,9 +26169,17 @@
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="C9" s="27">
+        <v>700</v>
+      </c>
+      <c r="D9" s="27">
+        <f t="shared" si="1"/>
+        <v>175</v>
+      </c>
+      <c r="E9" s="27">
+        <f t="shared" si="2"/>
+        <v>525</v>
+      </c>
       <c r="F9"/>
       <c r="O9" s="9"/>
       <c r="P9" s="8"/>
@@ -26023,9 +26193,20 @@
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="5" t="s">
+        <v>1580</v>
+      </c>
+      <c r="C10" s="27">
+        <v>240</v>
+      </c>
+      <c r="D10" s="27">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E10" s="27">
+        <f t="shared" si="2"/>
+        <v>180</v>
+      </c>
       <c r="F10"/>
       <c r="O10" s="9"/>
       <c r="P10" s="8"/>
@@ -26039,9 +26220,20 @@
       </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="A11" s="5" t="s">
+        <v>1581</v>
+      </c>
+      <c r="C11" s="27">
+        <v>284</v>
+      </c>
+      <c r="D11" s="27">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="E11" s="27">
+        <f t="shared" si="2"/>
+        <v>213</v>
+      </c>
       <c r="F11"/>
       <c r="O11" s="9"/>
       <c r="P11" s="8"/>
@@ -26055,9 +26247,20 @@
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="5" t="s">
+        <v>1582</v>
+      </c>
+      <c r="C12" s="27">
+        <v>195</v>
+      </c>
+      <c r="D12" s="27">
+        <f t="shared" si="1"/>
+        <v>48.75</v>
+      </c>
+      <c r="E12" s="27">
+        <f t="shared" si="2"/>
+        <v>146.25</v>
+      </c>
       <c r="F12"/>
       <c r="O12" s="9"/>
       <c r="P12" s="8"/>
@@ -26071,42 +26274,70 @@
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="5" t="s">
+        <v>1583</v>
+      </c>
+      <c r="C13" s="27">
+        <v>125</v>
+      </c>
+      <c r="D13" s="27">
+        <f t="shared" si="1"/>
+        <v>31.25</v>
+      </c>
+      <c r="E13" s="27">
+        <f t="shared" si="2"/>
+        <v>93.75</v>
+      </c>
       <c r="F13"/>
       <c r="O13" s="9"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="9"/>
       <c r="R13" s="8"/>
       <c r="S13" s="9"/>
-      <c r="U13" s="10"/>
+      <c r="U13" s="11"/>
       <c r="Z13" s="20" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14"/>
+      <c r="C14" s="27">
+        <v>1250</v>
+      </c>
+      <c r="D14" s="27">
+        <f t="shared" si="1"/>
+        <v>312.5</v>
+      </c>
+      <c r="E14" s="27">
+        <f t="shared" si="2"/>
+        <v>937.5</v>
+      </c>
       <c r="O14" s="9"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="9"/>
       <c r="R14" s="8"/>
       <c r="S14" s="9"/>
-      <c r="U14" s="11"/>
+      <c r="U14" s="10"/>
       <c r="Z14" s="20" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C15" s="27">
+        <v>175</v>
+      </c>
+      <c r="D15" s="27">
+        <f t="shared" si="1"/>
+        <v>43.75</v>
+      </c>
+      <c r="E15" s="27">
+        <f t="shared" si="2"/>
+        <v>131.25</v>
+      </c>
       <c r="O15" s="9"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="9"/>
-      <c r="R15" s="8"/>
       <c r="S15" s="9"/>
       <c r="U15" s="10"/>
       <c r="Z15" s="20" t="e">
@@ -26115,6 +26346,17 @@
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="C16" s="27">
+        <v>325</v>
+      </c>
+      <c r="D16" s="27">
+        <f t="shared" si="1"/>
+        <v>81.25</v>
+      </c>
+      <c r="E16" s="27">
+        <f t="shared" si="2"/>
+        <v>243.75</v>
+      </c>
       <c r="O16" s="9"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="9"/>
@@ -26129,6 +26371,7 @@
       <c r="O17" s="9"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="9"/>
+      <c r="R17" s="8"/>
       <c r="S17" s="9"/>
       <c r="U17" s="10"/>
       <c r="Z17" s="20" t="e">
@@ -26149,10 +26392,10 @@
       </c>
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="N19" s="9"/>
       <c r="O19" s="9"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="9"/>
-      <c r="R19" s="8"/>
       <c r="S19" s="9"/>
       <c r="U19" s="10"/>
       <c r="Z19" s="20" t="e">
@@ -26204,56 +26447,51 @@
       <c r="S23" s="9"/>
       <c r="U23" s="10"/>
       <c r="Z23" s="20" t="e">
-        <f t="shared" si="0"/>
+        <f>S23/G23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="N24" s="9"/>
-      <c r="O24" s="9"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="9"/>
-      <c r="S24" s="9"/>
-      <c r="U24" s="10"/>
-      <c r="Z24" s="20" t="e">
-        <f>S24/G24</f>
+    <row r="25" spans="2:26" x14ac:dyDescent="0.3">
+      <c r="G25" s="5">
+        <f>SUM(G2:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="S25" s="12">
+        <f>SUM(S2:S23)</f>
+        <v>0</v>
+      </c>
+      <c r="T25" s="20" t="e">
+        <f>S25/G25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="G26" s="5">
-        <f>SUM(G2:G24)</f>
-        <v>0</v>
-      </c>
-      <c r="S26" s="12">
-        <f>SUM(S2:S24)</f>
-        <v>0</v>
-      </c>
-      <c r="T26" s="20" t="e">
-        <f>S26/G26</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
     </row>
     <row r="27" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B27"/>
       <c r="C27"/>
       <c r="D27"/>
       <c r="E27"/>
-      <c r="F27"/>
-      <c r="G27"/>
+      <c r="G27" s="2"/>
       <c r="H27"/>
+      <c r="I27"/>
+      <c r="S27" s="2">
+        <v>62.5</v>
+      </c>
     </row>
     <row r="28" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
-      <c r="G28" s="2"/>
-      <c r="H28"/>
-      <c r="I28"/>
-      <c r="S28" s="2">
-        <v>62.5</v>
-      </c>
+      <c r="F28"/>
     </row>
     <row r="29" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B29"/>
@@ -26261,6 +26499,8 @@
       <c r="D29"/>
       <c r="E29"/>
       <c r="F29"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
     </row>
     <row r="30" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B30"/>
@@ -26268,20 +26508,11 @@
       <c r="D30"/>
       <c r="E30"/>
       <c r="F30"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="12"/>
-    </row>
-    <row r="31" spans="2:26" x14ac:dyDescent="0.3">
-      <c r="B31"/>
-      <c r="C31"/>
-      <c r="D31"/>
-      <c r="E31"/>
-      <c r="F31"/>
-      <c r="G31" s="12"/>
+      <c r="G30" s="12"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U24">
-    <sortCondition ref="O2:O24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U23">
+    <sortCondition ref="O2:O23"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -26529,10 +26760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I268"/>
+  <dimension ref="A1:I275"/>
   <sheetViews>
-    <sheetView topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="H269" sqref="H269"/>
+    <sheetView topLeftCell="A254" workbookViewId="0">
+      <selection activeCell="C275" sqref="C275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -30844,7 +31075,7 @@
         <v>30</v>
       </c>
       <c r="F205" s="24">
-        <f t="shared" ref="F205:F268" si="4">F204+E205-D205</f>
+        <f t="shared" ref="F205:F269" si="4">F204+E205-D205</f>
         <v>11168.400000000005</v>
       </c>
       <c r="G205" t="s">
@@ -32270,8 +32501,167 @@
         <v>104</v>
       </c>
     </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A269" s="23">
+        <v>45742</v>
+      </c>
+      <c r="B269" t="s">
+        <v>259</v>
+      </c>
+      <c r="C269" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E269">
+        <v>719</v>
+      </c>
+      <c r="F269" s="24">
+        <f t="shared" si="4"/>
+        <v>14783.550000000008</v>
+      </c>
+      <c r="G269" t="s">
+        <v>85</v>
+      </c>
+      <c r="H269" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A270" s="23">
+        <v>45742</v>
+      </c>
+      <c r="B270" t="s">
+        <v>259</v>
+      </c>
+      <c r="C270" t="s">
+        <v>1577</v>
+      </c>
+      <c r="E270">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="F270" s="24">
+        <f t="shared" ref="F270:F275" si="5">F269+E270-D270</f>
+        <v>14864.150000000009</v>
+      </c>
+      <c r="G270" t="s">
+        <v>145</v>
+      </c>
+      <c r="H270" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A271" s="23">
+        <v>45743</v>
+      </c>
+      <c r="B271" t="s">
+        <v>259</v>
+      </c>
+      <c r="C271" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E271">
+        <v>700</v>
+      </c>
+      <c r="F271" s="24">
+        <f t="shared" si="5"/>
+        <v>15564.150000000009</v>
+      </c>
+      <c r="G271" t="s">
+        <v>85</v>
+      </c>
+      <c r="H271" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A272" s="23">
+        <v>45744</v>
+      </c>
+      <c r="B272" t="s">
+        <v>264</v>
+      </c>
+      <c r="C272" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D272">
+        <v>15.59</v>
+      </c>
+      <c r="F272" s="24">
+        <f t="shared" si="5"/>
+        <v>15548.560000000009</v>
+      </c>
+      <c r="G272" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A273" s="23">
+        <v>45744</v>
+      </c>
+      <c r="B273" t="s">
+        <v>264</v>
+      </c>
+      <c r="C273" t="s">
+        <v>1002</v>
+      </c>
+      <c r="D273">
+        <v>15.59</v>
+      </c>
+      <c r="F273" s="24">
+        <f t="shared" si="5"/>
+        <v>15532.970000000008</v>
+      </c>
+      <c r="G273" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" s="23">
+        <v>45744</v>
+      </c>
+      <c r="B274" t="s">
+        <v>259</v>
+      </c>
+      <c r="C274" t="s">
+        <v>1584</v>
+      </c>
+      <c r="E274">
+        <v>125</v>
+      </c>
+      <c r="F274" s="24">
+        <f t="shared" si="5"/>
+        <v>15657.970000000008</v>
+      </c>
+      <c r="G274" t="s">
+        <v>85</v>
+      </c>
+      <c r="H274" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" s="23">
+        <v>45744</v>
+      </c>
+      <c r="B275" t="s">
+        <v>259</v>
+      </c>
+      <c r="C275" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E275">
+        <v>30</v>
+      </c>
+      <c r="F275" s="24">
+        <f t="shared" si="5"/>
+        <v>15687.970000000008</v>
+      </c>
+      <c r="G275" t="s">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I354" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
+  <autoFilter ref="A1:I353" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -34857,7 +35247,7 @@
   <dimension ref="A1:V242"/>
   <sheetViews>
     <sheetView topLeftCell="A222" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B243" sqref="B243"/>
+      <selection activeCell="A237" sqref="A237:XFD237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -37515,43 +37905,43 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>1111</v>
+        <v>1112</v>
       </c>
       <c r="B237" s="5" t="s">
-        <v>523</v>
+        <v>481</v>
       </c>
       <c r="C237" s="5" t="s">
-        <v>523</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>1112</v>
+        <v>1118</v>
       </c>
       <c r="B238" s="5" t="s">
-        <v>481</v>
+        <v>682</v>
       </c>
       <c r="C238" s="5" t="s">
-        <v>1113</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>1118</v>
+        <v>1311</v>
       </c>
       <c r="B239" s="5" t="s">
-        <v>682</v>
+        <v>1313</v>
       </c>
       <c r="C239" s="5" t="s">
-        <v>1120</v>
+        <v>466</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>1311</v>
+        <v>1312</v>
       </c>
       <c r="B240" s="5" t="s">
-        <v>1313</v>
+        <v>1314</v>
       </c>
       <c r="C240" s="5" t="s">
         <v>466</v>
@@ -37559,24 +37949,24 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>1312</v>
+        <v>1320</v>
       </c>
       <c r="B241" s="5" t="s">
-        <v>1314</v>
+        <v>481</v>
       </c>
       <c r="C241" s="5" t="s">
-        <v>466</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>1320</v>
+        <v>1585</v>
       </c>
       <c r="B242" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C242" s="5" t="s">
-        <v>1321</v>
+        <v>1586</v>
       </c>
     </row>
   </sheetData>
@@ -38056,24 +38446,20 @@
       <c r="A4" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="38">
+      <c r="B4">
         <v>6588.8800000000019</v>
       </c>
-      <c r="C4" s="38"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38">
+      <c r="C6">
         <v>240</v>
       </c>
     </row>
@@ -38081,8 +38467,7 @@
       <c r="A7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38">
+      <c r="C7">
         <v>245.4</v>
       </c>
     </row>
@@ -38090,8 +38475,7 @@
       <c r="A8" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38">
+      <c r="C8">
         <v>97.6</v>
       </c>
     </row>
@@ -38099,17 +38483,15 @@
       <c r="A9" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="38">
-        <v>30</v>
-      </c>
-      <c r="C9" s="38"/>
+      <c r="B9">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38">
+      <c r="C10">
         <v>200</v>
       </c>
     </row>
@@ -38117,8 +38499,7 @@
       <c r="A11" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38">
+      <c r="C11">
         <v>132</v>
       </c>
     </row>
@@ -38126,8 +38507,7 @@
       <c r="A12" s="26" t="s">
         <v>983</v>
       </c>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38">
+      <c r="C12">
         <v>210</v>
       </c>
     </row>
@@ -38135,8 +38515,7 @@
       <c r="A13" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38">
+      <c r="C13">
         <v>55.89</v>
       </c>
     </row>
@@ -38144,8 +38523,7 @@
       <c r="A14" s="26" t="s">
         <v>990</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38">
+      <c r="C14">
         <v>625</v>
       </c>
     </row>
@@ -38153,35 +38531,31 @@
       <c r="A15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38">
-        <v>7.95</v>
+      <c r="C15">
+        <v>39.129999999999995</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="38">
+      <c r="B16">
         <v>1.77</v>
       </c>
-      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="38">
+      <c r="B17">
         <v>2443.5299999999997</v>
       </c>
-      <c r="C17" s="38"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38">
+      <c r="C18">
         <v>606.6</v>
       </c>
     </row>
@@ -38189,10 +38563,10 @@
       <c r="A19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="38">
-        <v>159.37</v>
-      </c>
-      <c r="C19" s="38">
+      <c r="B19">
+        <v>239.97</v>
+      </c>
+      <c r="C19">
         <v>30</v>
       </c>
     </row>
@@ -38200,8 +38574,7 @@
       <c r="A20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38">
+      <c r="C20">
         <v>200</v>
       </c>
     </row>
@@ -38209,8 +38582,7 @@
       <c r="A21" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38">
+      <c r="C21">
         <v>613.22</v>
       </c>
     </row>
@@ -38218,20 +38590,19 @@
       <c r="A22" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="38">
-        <v>2280.7800000000002</v>
-      </c>
-      <c r="C22" s="38"/>
+      <c r="B22">
+        <v>3824.78</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="38">
-        <v>11504.330000000004</v>
-      </c>
-      <c r="C23" s="38">
-        <v>3263.66</v>
+      <c r="B23">
+        <v>13128.930000000002</v>
+      </c>
+      <c r="C23">
+        <v>3294.84</v>
       </c>
     </row>
   </sheetData>
@@ -38243,8 +38614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FA1291-B9CE-4F7D-8600-2336ADED0E75}">
   <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -38254,7 +38625,7 @@
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>106</v>
       </c>
@@ -38262,7 +38633,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>82</v>
       </c>
@@ -38273,86 +38644,74 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38">
+      <c r="C4">
         <v>25.4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38">
+      <c r="C5">
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38">
+      <c r="C6">
         <v>431.6</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="38">
+      <c r="B7">
         <v>2443.5300000000007</v>
       </c>
-      <c r="C7" s="38"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38">
+      <c r="C8">
         <v>245.4</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="38">
-        <v>159.37</v>
-      </c>
-      <c r="C9" s="38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>239.97</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="38">
-        <v>2280.7800000000002</v>
-      </c>
-      <c r="C10" s="38"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>3824.78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="38">
-        <v>4883.68</v>
-      </c>
-      <c r="C11" s="38">
+      <c r="B11">
+        <v>6508.2800000000007</v>
+      </c>
+      <c r="C11">
         <v>932.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I12">
-        <f>7695.3-7590.3</f>
-        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -38395,8 +38754,7 @@
       <c r="A20" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="38"/>
-      <c r="C20" s="38">
+      <c r="C20">
         <v>132</v>
       </c>
       <c r="E20" t="s">
@@ -38416,10 +38774,9 @@
       <c r="A21" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="38">
-        <v>30</v>
-      </c>
-      <c r="C21" s="38"/>
+      <c r="B21">
+        <v>30</v>
+      </c>
       <c r="E21" t="s">
         <v>117</v>
       </c>
@@ -38434,8 +38791,7 @@
       <c r="A22" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38">
+      <c r="C22">
         <v>200</v>
       </c>
       <c r="E22" t="s">
@@ -38454,8 +38810,7 @@
       <c r="A23" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38">
+      <c r="C23">
         <v>30.49</v>
       </c>
     </row>
@@ -38463,8 +38818,7 @@
       <c r="A24" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38">
+      <c r="C24">
         <v>613.22</v>
       </c>
     </row>
@@ -38472,8 +38826,7 @@
       <c r="A25" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="38">
+      <c r="C25">
         <v>175</v>
       </c>
     </row>
@@ -38481,8 +38834,7 @@
       <c r="A26" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="38">
+      <c r="C26">
         <v>240</v>
       </c>
     </row>
@@ -38490,33 +38842,28 @@
       <c r="A27" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="38">
-        <v>7.95</v>
+      <c r="C27">
+        <v>39.129999999999995</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="38">
+      <c r="B29">
         <v>1.77</v>
       </c>
-      <c r="C29" s="38"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38">
+      <c r="C30">
         <v>97.6</v>
       </c>
     </row>
@@ -38524,17 +38871,15 @@
       <c r="A31" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B31" s="38">
+      <c r="B31">
         <v>6588.8800000000019</v>
       </c>
-      <c r="C31" s="38"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="26" t="s">
         <v>983</v>
       </c>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38">
+      <c r="C32">
         <v>210</v>
       </c>
     </row>
@@ -38542,8 +38887,7 @@
       <c r="A33" s="26" t="s">
         <v>990</v>
       </c>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38">
+      <c r="C33">
         <v>625</v>
       </c>
     </row>
@@ -38551,11 +38895,11 @@
       <c r="A34" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="38">
+      <c r="B34">
         <v>6620.6500000000024</v>
       </c>
-      <c r="C34" s="38">
-        <v>2331.2600000000002</v>
+      <c r="C34">
+        <v>2362.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Young Artists exhibition
</commit_message>
<xml_diff>
--- a/OAS 2025.xlsx
+++ b/OAS 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1427F50D-C19A-4C3D-B826-0C3E0C6E943D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973BFD9A-5255-4DD1-9EF7-1982798E01E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="1" activeTab="1" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4264" uniqueCount="1658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4323" uniqueCount="1669">
   <si>
     <t>Subs</t>
   </si>
@@ -4936,9 +4936,6 @@
     <t>Artist paid</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -5033,6 +5030,42 @@
   </si>
   <si>
     <t>Philip Vainker OAS</t>
+  </si>
+  <si>
+    <t>Susan Wheeler OAS</t>
+  </si>
+  <si>
+    <t>Vivian Shelton OAS</t>
+  </si>
+  <si>
+    <t>Deborah Williams OAS</t>
+  </si>
+  <si>
+    <t>GROSS INTEREST TO 16APR2025</t>
+  </si>
+  <si>
+    <t>TOTAL CHARGES TO 30MAR2025</t>
+  </si>
+  <si>
+    <t>Stripe OAS</t>
+  </si>
+  <si>
+    <t>Committee meeting refreshments</t>
+  </si>
+  <si>
+    <t>Roberta Catizone OAS</t>
+  </si>
+  <si>
+    <t>Commision on direct sale</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>Erin Thomas OAS</t>
+  </si>
+  <si>
+    <t>Young artists</t>
   </si>
 </sst>
 </file>
@@ -5290,13 +5323,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45761.461562268516" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="299" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45786.524010532405" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="315" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I400" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-04-15T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-05-10T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5305,7 +5338,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Expenditure" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="937.5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="1500"/>
     </cacheField>
     <cacheField name="Income" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
@@ -5314,7 +5347,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="18411.630000000008"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
-      <sharedItems containsBlank="1" count="21">
+      <sharedItems containsBlank="1" count="23">
         <m/>
         <s v="Subs 2025"/>
         <s v="Donations cr"/>
@@ -5335,6 +5368,8 @@
         <s v="Insurance"/>
         <s v="Sales cr"/>
         <s v="Sales db"/>
+        <s v="Exhibition organisers fees"/>
+        <s v="Website manager's fee"/>
         <s v="Exhibitions cr" u="1"/>
       </sharedItems>
     </cacheField>
@@ -5354,13 +5389,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45761.461653356484" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="299" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45786.524056249997" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="315" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I503" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-04-15T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-05-10T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5369,7 +5404,7 @@
       <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Expenditure" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="937.5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5" maxValue="1500"/>
     </cacheField>
     <cacheField name="Income" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
@@ -5399,11 +5434,11 @@
         <s v="Insurance"/>
         <s v="Sales cr"/>
         <s v="Sales db"/>
+        <s v="Exhibition organisers fees"/>
+        <s v="Website manager's fee"/>
         <s v="Exhibitions cr" u="1"/>
         <s v="Subs" u="1"/>
         <s v="Admin" u="1"/>
-        <s v="Website manager's fee" u="1"/>
-        <s v="Exhibition organisers fees" u="1"/>
         <s v="Prof Fees" u="1"/>
         <s v="Venue hire" u="1"/>
         <s v="Transfer Out" u="1"/>
@@ -5411,9 +5446,10 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Exhibition" numFmtId="0">
-      <sharedItems containsBlank="1" count="3">
+      <sharedItems containsBlank="1" count="4">
         <m/>
         <s v="Members"/>
+        <s v="Young artists"/>
         <s v="Open" u="1"/>
       </sharedItems>
     </cacheField>
@@ -5430,7 +5466,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="299">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="315">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -8710,6 +8746,182 @@
     <m/>
   </r>
   <r>
+    <d v="2025-04-15T00:00:00"/>
+    <s v="BP"/>
+    <s v="Susan Wheeler OAS"/>
+    <n v="281.25"/>
+    <m/>
+    <n v="14323.500000000007"/>
+    <x v="19"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="750"/>
+    <m/>
+    <n v="13573.500000000007"/>
+    <x v="20"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="43.17"/>
+    <m/>
+    <n v="13530.330000000007"/>
+    <x v="4"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-18T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="124.65"/>
+    <m/>
+    <n v="13405.680000000008"/>
+    <x v="4"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-18T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="750"/>
+    <m/>
+    <n v="12655.680000000008"/>
+    <x v="20"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-21T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="66.790000000000006"/>
+    <m/>
+    <n v="12588.890000000007"/>
+    <x v="4"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-21T00:00:00"/>
+    <s v="CHG"/>
+    <s v="TOTAL CHARGES TO 30MAR2025"/>
+    <n v="5.72"/>
+    <m/>
+    <n v="12583.170000000007"/>
+    <x v="5"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Jill Colchester OAS"/>
+    <n v="213"/>
+    <m/>
+    <n v="12370.170000000007"/>
+    <x v="19"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Stripe OAS"/>
+    <n v="15"/>
+    <m/>
+    <n v="12355.170000000007"/>
+    <x v="3"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Rebecca Payton OAS"/>
+    <n v="17.75"/>
+    <m/>
+    <n v="12337.420000000007"/>
+    <x v="5"/>
+    <m/>
+    <s v="Committee meeting refreshments"/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="Split"/>
+    <s v="Roberta Catizone OAS"/>
+    <n v="1500"/>
+    <m/>
+    <n v="10837.420000000007"/>
+    <x v="21"/>
+    <s v="Members"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="Split"/>
+    <s v="Roberta Catizone OAS"/>
+    <n v="264.14999999999998"/>
+    <m/>
+    <n v="10573.270000000008"/>
+    <x v="11"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-25T00:00:00"/>
+    <s v="CR"/>
+    <s v="Olding Alexandra ALEXANDRA BUCKLE"/>
+    <m/>
+    <n v="47.5"/>
+    <n v="10620.770000000008"/>
+    <x v="18"/>
+    <s v="Members"/>
+    <s v="Commision on direct sale"/>
+  </r>
+  <r>
+    <d v="2025-05-01T00:00:00"/>
+    <s v="SO"/>
+    <s v="Jeremy Morgan OAS"/>
+    <n v="240"/>
+    <m/>
+    <n v="10380.770000000008"/>
+    <x v="8"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="41.42"/>
+    <m/>
+    <n v="10339.350000000008"/>
+    <x v="14"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="122.1"/>
+    <m/>
+    <n v="10217.250000000007"/>
+    <x v="20"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -8724,7 +8936,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="299">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="315">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -12001,6 +12213,182 @@
     <n v="14604.750000000007"/>
     <x v="19"/>
     <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-15T00:00:00"/>
+    <s v="BP"/>
+    <s v="Susan Wheeler OAS"/>
+    <n v="281.25"/>
+    <m/>
+    <n v="14323.500000000007"/>
+    <x v="19"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="750"/>
+    <m/>
+    <n v="13573.500000000007"/>
+    <x v="20"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Vivian Shelton OAS"/>
+    <n v="43.17"/>
+    <m/>
+    <n v="13530.330000000007"/>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-18T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="124.65"/>
+    <m/>
+    <n v="13405.680000000008"/>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-18T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="750"/>
+    <m/>
+    <n v="12655.680000000008"/>
+    <x v="20"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-21T00:00:00"/>
+    <s v="BP"/>
+    <s v="Deborah Williams OAS"/>
+    <n v="66.790000000000006"/>
+    <m/>
+    <n v="12588.890000000007"/>
+    <x v="4"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-21T00:00:00"/>
+    <s v="CHG"/>
+    <s v="TOTAL CHARGES TO 30MAR2025"/>
+    <n v="5.72"/>
+    <m/>
+    <n v="12583.170000000007"/>
+    <x v="5"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Jill Colchester OAS"/>
+    <n v="213"/>
+    <m/>
+    <n v="12370.170000000007"/>
+    <x v="19"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Stripe OAS"/>
+    <n v="15"/>
+    <m/>
+    <n v="12355.170000000007"/>
+    <x v="3"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="BP"/>
+    <s v="Rebecca Payton OAS"/>
+    <n v="17.75"/>
+    <m/>
+    <n v="12337.420000000007"/>
+    <x v="5"/>
+    <x v="0"/>
+    <s v="Committee meeting refreshments"/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="Split"/>
+    <s v="Roberta Catizone OAS"/>
+    <n v="1500"/>
+    <m/>
+    <n v="10837.420000000007"/>
+    <x v="21"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-24T00:00:00"/>
+    <s v="Split"/>
+    <s v="Roberta Catizone OAS"/>
+    <n v="264.14999999999998"/>
+    <m/>
+    <n v="10573.270000000008"/>
+    <x v="11"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-04-25T00:00:00"/>
+    <s v="CR"/>
+    <s v="Olding Alexandra ALEXANDRA BUCKLE"/>
+    <m/>
+    <n v="47.5"/>
+    <n v="10620.770000000008"/>
+    <x v="18"/>
+    <x v="1"/>
+    <s v="Commision on direct sale"/>
+  </r>
+  <r>
+    <d v="2025-05-01T00:00:00"/>
+    <s v="SO"/>
+    <s v="Jeremy Morgan OAS"/>
+    <n v="240"/>
+    <m/>
+    <n v="10380.770000000008"/>
+    <x v="8"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="41.42"/>
+    <m/>
+    <n v="10339.350000000008"/>
+    <x v="14"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-05-09T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="122.1"/>
+    <m/>
+    <n v="10217.250000000007"/>
+    <x v="20"/>
+    <x v="2"/>
     <m/>
   </r>
   <r>
@@ -12019,7 +12407,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB64E1A4-8455-499E-80FF-BC0BFCCF7279}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C24" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A3:C26" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -12028,7 +12416,7 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="22">
+      <items count="24">
         <item x="1"/>
         <item x="0"/>
         <item x="3"/>
@@ -12047,9 +12435,11 @@
         <item x="15"/>
         <item x="16"/>
         <item x="17"/>
-        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item x="18"/>
         <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12059,7 +12449,7 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="21">
+  <rowItems count="23">
     <i>
       <x/>
     </i>
@@ -12120,6 +12510,12 @@
     <i>
       <x v="20"/>
     </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -12153,7 +12549,7 @@
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A3:C15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -12163,11 +12559,11 @@
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="30">
-        <item m="1" x="22"/>
+        <item m="1" x="24"/>
         <item x="7"/>
         <item x="2"/>
         <item x="6"/>
-        <item m="1" x="24"/>
+        <item x="20"/>
         <item x="9"/>
         <item x="17"/>
         <item x="16"/>
@@ -12177,7 +12573,7 @@
         <item x="18"/>
         <item x="19"/>
         <item x="13"/>
-        <item m="1" x="21"/>
+        <item m="1" x="23"/>
         <item x="11"/>
         <item m="1" x="26"/>
         <item x="0"/>
@@ -12187,19 +12583,20 @@
         <item x="5"/>
         <item x="15"/>
         <item m="1" x="27"/>
-        <item m="1" x="23"/>
+        <item x="21"/>
         <item x="1"/>
         <item x="8"/>
         <item x="10"/>
-        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="4">
+      <items count="5">
         <item x="1"/>
-        <item m="1" x="2"/>
+        <item m="1" x="3"/>
         <item x="0"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12208,7 +12605,10 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="12">
+    <i>
+      <x v="4"/>
+    </i>
     <i>
       <x v="5"/>
     </i>
@@ -12217,6 +12617,9 @@
     </i>
     <i>
       <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
     </i>
     <i>
       <x v="11"/>
@@ -12232,6 +12635,9 @@
     </i>
     <i>
       <x v="22"/>
+    </i>
+    <i>
+      <x v="24"/>
     </i>
     <i t="grand">
       <x/>
@@ -12269,7 +12675,7 @@
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A19:C34" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <location ref="A19:C22" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -12279,11 +12685,11 @@
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="30">
-        <item m="1" x="22"/>
+        <item m="1" x="24"/>
         <item x="7"/>
         <item x="2"/>
         <item x="6"/>
-        <item m="1" x="24"/>
+        <item x="20"/>
         <item x="9"/>
         <item x="17"/>
         <item x="16"/>
@@ -12293,7 +12699,7 @@
         <item x="18"/>
         <item x="19"/>
         <item x="13"/>
-        <item m="1" x="21"/>
+        <item m="1" x="23"/>
         <item x="11"/>
         <item m="1" x="26"/>
         <item x="0"/>
@@ -12303,19 +12709,20 @@
         <item x="5"/>
         <item x="15"/>
         <item m="1" x="27"/>
-        <item m="1" x="23"/>
+        <item x="21"/>
         <item x="1"/>
         <item x="8"/>
         <item x="10"/>
-        <item m="1" x="20"/>
+        <item m="1" x="22"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisPage" showAll="0">
-      <items count="4">
+      <items count="5">
         <item x="1"/>
-        <item m="1" x="2"/>
+        <item m="1" x="3"/>
         <item x="0"/>
+        <item x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -12324,48 +12731,12 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="15">
+  <rowItems count="3">
     <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
+      <x v="4"/>
     </i>
     <i>
       <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
     </i>
     <i t="grand">
       <x/>
@@ -12383,7 +12754,7 @@
     </i>
   </colItems>
   <pageFields count="1">
-    <pageField fld="7" item="2" hier="-1"/>
+    <pageField fld="7" item="3" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
@@ -12831,7 +13202,7 @@
       </c>
       <c r="C5" s="31">
         <f>GETPIVOTDATA("Sum of Income",Exhibitions!$A$3,"Category","Sales cr")</f>
-        <v>8167.8099999999995</v>
+        <v>8215.31</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17" t="s">
@@ -12868,15 +13239,15 @@
       <c r="B6" s="16"/>
       <c r="C6" s="34">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Sales db")</f>
-        <v>5426.25</v>
+        <v>5920.5</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="F6" s="31" t="e">
+      <c r="F6" s="31">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Website manager's fee")</f>
-        <v>#REF!</v>
+        <v>1500</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -12903,15 +13274,15 @@
       <c r="B7" s="16"/>
       <c r="C7" s="31">
         <f>C5-C6</f>
-        <v>2741.5599999999995</v>
+        <v>2294.8099999999995</v>
       </c>
       <c r="D7" s="21"/>
       <c r="E7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="31" t="e">
+      <c r="F7" s="31">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Exhibition organisers fees")</f>
-        <v>#REF!</v>
+        <v>1500</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -12921,7 +13292,7 @@
       <c r="J7" s="17"/>
       <c r="K7" s="31">
         <f>SUMIF('Savings account'!G2:G15, "Interest", 'Savings account'!E2:E15)</f>
-        <v>101.69</v>
+        <v>135.74</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="17" t="s">
@@ -12930,7 +13301,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="31">
         <f>SUMIF('Current account'!G2:G401,"Admin",'Current account'!D2:D401)+SUMIF('Current account'!G2:G401, "Other expenses", 'Current account'!D2:D401)</f>
-        <v>97.6</v>
+        <v>121.07</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
@@ -12955,7 +13326,7 @@
       <c r="N8" s="17"/>
       <c r="O8" s="31">
         <f ca="1">SUMIF('Current account'!G2:G401,"Website",'Current account'!D2:D41)</f>
-        <v>39.129999999999995</v>
+        <v>303.27999999999997</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.4">
@@ -13003,9 +13374,9 @@
       <c r="E10" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="31" t="e">
+      <c r="F10" s="31">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Refunds")</f>
-        <v>#REF!</v>
+        <v>15</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -13142,7 +13513,7 @@
       <c r="N15" s="17"/>
       <c r="O15" s="31">
         <f ca="1">SUM(O4:O13)</f>
-        <v>1137.8400000000001</v>
+        <v>1425.46</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -16631,7 +17002,7 @@
         <v>45752.486319444448</v>
       </c>
       <c r="C59" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D59" t="s">
         <v>1460</v>
@@ -16643,7 +17014,7 @@
         <v>1462</v>
       </c>
       <c r="G59" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="H59" t="s">
         <v>1469</v>
@@ -16655,7 +17026,7 @@
         <v>1470</v>
       </c>
       <c r="K59" s="42" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="M59">
         <v>360</v>
@@ -16685,7 +17056,7 @@
         <v>45752.559618055559</v>
       </c>
       <c r="C60" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D60" t="s">
         <v>1460</v>
@@ -16697,7 +17068,7 @@
         <v>1462</v>
       </c>
       <c r="G60" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="H60" t="s">
         <v>1469</v>
@@ -16739,7 +17110,7 @@
         <v>45752.713935185187</v>
       </c>
       <c r="C61" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="D61" t="s">
         <v>1460</v>
@@ -16751,7 +17122,7 @@
         <v>1462</v>
       </c>
       <c r="G61" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="H61" t="s">
         <v>1464</v>
@@ -16763,7 +17134,7 @@
         <v>1470</v>
       </c>
       <c r="K61" s="42" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="M61">
         <v>375</v>
@@ -27023,7 +27394,7 @@
   <dimension ref="A1:Z30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -27068,7 +27439,7 @@
         <v>1611</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>1624</v>
@@ -27099,7 +27470,7 @@
         <v>1616</v>
       </c>
       <c r="H2" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O2" s="9"/>
       <c r="P2" s="8"/>
@@ -27137,7 +27508,7 @@
         <v>1616</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O3" s="9"/>
       <c r="P3" s="8"/>
@@ -27179,7 +27550,7 @@
         <v>1612</v>
       </c>
       <c r="H4" s="41" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="8"/>
@@ -27216,7 +27587,7 @@
         <v>148</v>
       </c>
       <c r="H5" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O5" s="9"/>
       <c r="P5" s="8"/>
@@ -27253,7 +27624,7 @@
         <v>1616</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O6" s="9"/>
       <c r="P6" s="8"/>
@@ -27291,7 +27662,7 @@
         <v>1616</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="8"/>
@@ -27367,7 +27738,7 @@
         <v>1616</v>
       </c>
       <c r="H9" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O9" s="9"/>
       <c r="P9" s="8"/>
@@ -27405,7 +27776,7 @@
         <v>1616</v>
       </c>
       <c r="H10" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O10" s="9"/>
       <c r="P10" s="8"/>
@@ -27443,7 +27814,7 @@
         <v>1616</v>
       </c>
       <c r="H11" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O11" s="9"/>
       <c r="P11" s="8"/>
@@ -27481,7 +27852,7 @@
         <v>1616</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O12" s="9"/>
       <c r="P12" s="8"/>
@@ -27519,7 +27890,7 @@
         <v>1616</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O13" s="9"/>
       <c r="P13" s="8"/>
@@ -27557,7 +27928,7 @@
         <v>1616</v>
       </c>
       <c r="H14" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O14" s="9"/>
       <c r="P14" s="8"/>
@@ -27595,7 +27966,7 @@
         <v>1617</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O15" s="9"/>
       <c r="P15" s="8"/>
@@ -27632,7 +28003,7 @@
         <v>1617</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O16" s="9"/>
       <c r="P16" s="8"/>
@@ -27669,7 +28040,7 @@
         <v>1617</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="8"/>
@@ -27707,7 +28078,7 @@
         <v>1617</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="O18" s="9"/>
       <c r="P18" s="8"/>
@@ -27745,7 +28116,7 @@
         <v>1616</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
@@ -27783,7 +28154,7 @@
         <v>1616</v>
       </c>
       <c r="H20" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="N20" s="9"/>
       <c r="O20" s="9"/>
@@ -27821,7 +28192,7 @@
         <v>1616</v>
       </c>
       <c r="H21" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
@@ -27859,7 +28230,7 @@
         <v>1617</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
@@ -27897,7 +28268,7 @@
         <v>1616</v>
       </c>
       <c r="H23" s="40" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
@@ -28060,8 +28431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0167813-1C3C-42CC-A5D8-7CCC1B587009}">
   <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -28102,6 +28473,9 @@
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="B5" t="s">
+        <v>1668</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -28241,10 +28615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I299"/>
+  <dimension ref="A1:I315"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A276" workbookViewId="0">
-      <selection activeCell="H300" sqref="H300"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="A316" sqref="A316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -34020,7 +34394,7 @@
         <v>80.599999999999994</v>
       </c>
       <c r="F270" s="24">
-        <f t="shared" ref="F270:F299" si="5">F269+E270-D270</f>
+        <f t="shared" ref="F270:F315" si="5">F269+E270-D270</f>
         <v>14864.150000000009</v>
       </c>
       <c r="G270" t="s">
@@ -34221,7 +34595,7 @@
         <v>264</v>
       </c>
       <c r="C279" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D279">
         <v>90</v>
@@ -34245,7 +34619,7 @@
         <v>264</v>
       </c>
       <c r="C280" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="E280">
         <v>375</v>
@@ -34261,7 +34635,7 @@
         <v>104</v>
       </c>
       <c r="I280" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.35">
@@ -34272,7 +34646,7 @@
         <v>264</v>
       </c>
       <c r="C281" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D281">
         <v>187.5</v>
@@ -34296,7 +34670,7 @@
         <v>264</v>
       </c>
       <c r="C282" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="D282">
         <v>270</v>
@@ -34320,7 +34694,7 @@
         <v>264</v>
       </c>
       <c r="C283" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="D283">
         <v>431.25</v>
@@ -34344,7 +34718,7 @@
         <v>264</v>
       </c>
       <c r="C284" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="D284">
         <v>180</v>
@@ -34368,7 +34742,7 @@
         <v>264</v>
       </c>
       <c r="C285" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
       <c r="D285">
         <v>138.75</v>
@@ -34392,7 +34766,7 @@
         <v>264</v>
       </c>
       <c r="C286" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="D286">
         <v>525</v>
@@ -34416,7 +34790,7 @@
         <v>264</v>
       </c>
       <c r="C287" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="D287">
         <v>450</v>
@@ -34440,7 +34814,7 @@
         <v>264</v>
       </c>
       <c r="C288" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="D288">
         <v>543.75</v>
@@ -34464,7 +34838,7 @@
         <v>264</v>
       </c>
       <c r="C289" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="D289">
         <v>146.25</v>
@@ -34488,7 +34862,7 @@
         <v>264</v>
       </c>
       <c r="C290" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="D290">
         <v>180</v>
@@ -34512,7 +34886,7 @@
         <v>264</v>
       </c>
       <c r="C291" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D291">
         <v>337.5</v>
@@ -34536,7 +34910,7 @@
         <v>264</v>
       </c>
       <c r="C292" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D292">
         <v>131.25</v>
@@ -34560,7 +34934,7 @@
         <v>259</v>
       </c>
       <c r="C293" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="E293">
         <v>1086.32</v>
@@ -34584,7 +34958,7 @@
         <v>264</v>
       </c>
       <c r="C294" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D294">
         <v>108.75</v>
@@ -34632,7 +35006,7 @@
         <v>264</v>
       </c>
       <c r="C296" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D296">
         <v>937.5</v>
@@ -34656,7 +35030,7 @@
         <v>264</v>
       </c>
       <c r="C297" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D297">
         <v>281.25</v>
@@ -34680,7 +35054,7 @@
         <v>264</v>
       </c>
       <c r="C298" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="D298">
         <v>337.5</v>
@@ -34704,7 +35078,7 @@
         <v>264</v>
       </c>
       <c r="C299" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="D299">
         <v>150</v>
@@ -34720,9 +35094,388 @@
         <v>104</v>
       </c>
     </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A300" s="23">
+        <v>45762</v>
+      </c>
+      <c r="B300" t="s">
+        <v>264</v>
+      </c>
+      <c r="C300" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D300">
+        <v>281.25</v>
+      </c>
+      <c r="F300" s="24">
+        <f t="shared" si="5"/>
+        <v>14323.500000000007</v>
+      </c>
+      <c r="G300" t="s">
+        <v>87</v>
+      </c>
+      <c r="H300" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A301" s="23">
+        <v>45763</v>
+      </c>
+      <c r="B301" t="s">
+        <v>264</v>
+      </c>
+      <c r="C301" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D301">
+        <v>750</v>
+      </c>
+      <c r="F301" s="24">
+        <f t="shared" si="5"/>
+        <v>13573.500000000007</v>
+      </c>
+      <c r="G301" t="s">
+        <v>103</v>
+      </c>
+      <c r="H301" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A302" s="23">
+        <v>45763</v>
+      </c>
+      <c r="B302" t="s">
+        <v>264</v>
+      </c>
+      <c r="C302" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D302">
+        <v>43.17</v>
+      </c>
+      <c r="F302" s="24">
+        <f t="shared" si="5"/>
+        <v>13530.330000000007</v>
+      </c>
+      <c r="G302" t="s">
+        <v>89</v>
+      </c>
+      <c r="H302" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A303" s="23">
+        <v>45765</v>
+      </c>
+      <c r="B303" t="s">
+        <v>264</v>
+      </c>
+      <c r="C303" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D303">
+        <v>124.65</v>
+      </c>
+      <c r="F303" s="24">
+        <f t="shared" si="5"/>
+        <v>13405.680000000008</v>
+      </c>
+      <c r="G303" t="s">
+        <v>89</v>
+      </c>
+      <c r="H303" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A304" s="23">
+        <v>45765</v>
+      </c>
+      <c r="B304" t="s">
+        <v>264</v>
+      </c>
+      <c r="C304" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D304">
+        <v>750</v>
+      </c>
+      <c r="F304" s="24">
+        <f t="shared" si="5"/>
+        <v>12655.680000000008</v>
+      </c>
+      <c r="G304" t="s">
+        <v>103</v>
+      </c>
+      <c r="H304" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A305" s="23">
+        <v>45768</v>
+      </c>
+      <c r="B305" t="s">
+        <v>264</v>
+      </c>
+      <c r="C305" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D305">
+        <v>66.790000000000006</v>
+      </c>
+      <c r="F305" s="24">
+        <f t="shared" si="5"/>
+        <v>12588.890000000007</v>
+      </c>
+      <c r="G305" t="s">
+        <v>89</v>
+      </c>
+      <c r="H305" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A306" s="23">
+        <v>45768</v>
+      </c>
+      <c r="B306" t="s">
+        <v>782</v>
+      </c>
+      <c r="C306" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D306">
+        <v>5.72</v>
+      </c>
+      <c r="F306" s="24">
+        <f t="shared" si="5"/>
+        <v>12583.170000000007</v>
+      </c>
+      <c r="G306" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A307" s="23">
+        <v>45771</v>
+      </c>
+      <c r="B307" t="s">
+        <v>264</v>
+      </c>
+      <c r="C307" t="s">
+        <v>807</v>
+      </c>
+      <c r="D307">
+        <v>213</v>
+      </c>
+      <c r="F307" s="24">
+        <f t="shared" si="5"/>
+        <v>12370.170000000007</v>
+      </c>
+      <c r="G307" t="s">
+        <v>87</v>
+      </c>
+      <c r="H307" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A308" s="23">
+        <v>45771</v>
+      </c>
+      <c r="B308" t="s">
+        <v>264</v>
+      </c>
+      <c r="C308" t="s">
+        <v>1662</v>
+      </c>
+      <c r="D308">
+        <v>15</v>
+      </c>
+      <c r="F308" s="24">
+        <f t="shared" si="5"/>
+        <v>12355.170000000007</v>
+      </c>
+      <c r="G308" t="s">
+        <v>5</v>
+      </c>
+      <c r="H308" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A309" s="23">
+        <v>45771</v>
+      </c>
+      <c r="B309" t="s">
+        <v>264</v>
+      </c>
+      <c r="C309" t="s">
+        <v>725</v>
+      </c>
+      <c r="D309">
+        <v>17.75</v>
+      </c>
+      <c r="F309" s="24">
+        <f t="shared" si="5"/>
+        <v>12337.420000000007</v>
+      </c>
+      <c r="G309" t="s">
+        <v>113</v>
+      </c>
+      <c r="I309" t="s">
+        <v>1663</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A310" s="23">
+        <v>45771</v>
+      </c>
+      <c r="B310" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C310" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D310">
+        <v>1500</v>
+      </c>
+      <c r="F310" s="24">
+        <f t="shared" si="5"/>
+        <v>10837.420000000007</v>
+      </c>
+      <c r="G310" t="s">
+        <v>170</v>
+      </c>
+      <c r="H310" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A311" s="23">
+        <v>45771</v>
+      </c>
+      <c r="B311" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C311" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D311">
+        <v>264.14999999999998</v>
+      </c>
+      <c r="F311" s="24">
+        <f t="shared" si="5"/>
+        <v>10573.270000000008</v>
+      </c>
+      <c r="G311" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A312" s="23">
+        <v>45772</v>
+      </c>
+      <c r="B312" t="s">
+        <v>259</v>
+      </c>
+      <c r="C312" t="s">
+        <v>192</v>
+      </c>
+      <c r="E312">
+        <v>47.5</v>
+      </c>
+      <c r="F312" s="24">
+        <f t="shared" si="5"/>
+        <v>10620.770000000008</v>
+      </c>
+      <c r="G312" t="s">
+        <v>86</v>
+      </c>
+      <c r="H312" t="s">
+        <v>104</v>
+      </c>
+      <c r="I312" t="s">
+        <v>1665</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A313" s="23">
+        <v>45778</v>
+      </c>
+      <c r="B313" t="s">
+        <v>1666</v>
+      </c>
+      <c r="C313" t="s">
+        <v>982</v>
+      </c>
+      <c r="D313">
+        <v>240</v>
+      </c>
+      <c r="F313" s="24">
+        <f t="shared" si="5"/>
+        <v>10380.770000000008</v>
+      </c>
+      <c r="G313" t="s">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A314" s="23">
+        <v>45786</v>
+      </c>
+      <c r="B314" t="s">
+        <v>264</v>
+      </c>
+      <c r="C314" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D314">
+        <v>41.42</v>
+      </c>
+      <c r="F314" s="24">
+        <f t="shared" si="5"/>
+        <v>10339.350000000008</v>
+      </c>
+      <c r="G314" t="s">
+        <v>49</v>
+      </c>
+      <c r="H314" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A315" s="23">
+        <v>45786</v>
+      </c>
+      <c r="B315" t="s">
+        <v>264</v>
+      </c>
+      <c r="C315" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D315">
+        <v>122.1</v>
+      </c>
+      <c r="F315" s="24">
+        <f t="shared" si="5"/>
+        <v>10217.250000000007</v>
+      </c>
+      <c r="G315" t="s">
+        <v>103</v>
+      </c>
+      <c r="H315" t="s">
+        <v>1668</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I353" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -34732,11 +35485,11 @@
           </x14:formula1>
           <xm:sqref>G1:G190 G192:G195 G197:G1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E82AE568-40FA-4E8D-9A51-0EEEFCB67DE0}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5FBF1F7E-70E4-4F92-A226-94216AF53046}">
           <x14:formula1>
-            <xm:f>Lists!$B$3:$B$4</xm:f>
+            <xm:f>Lists!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -34749,10 +35502,10 @@
   <dimension ref="A1:Y349"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C248" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B291" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D268" sqref="D268"/>
+      <selection pane="bottomRight" activeCell="A303" sqref="A303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -37590,7 +38343,7 @@
         <v>15.59</v>
       </c>
     </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A273" s="23">
         <v>45744</v>
       </c>
@@ -37598,7 +38351,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A274" s="23">
         <v>45744</v>
       </c>
@@ -37606,7 +38359,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A275" s="23">
         <v>45746</v>
       </c>
@@ -37614,7 +38367,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A276" s="23">
         <v>45747</v>
       </c>
@@ -37622,12 +38375,308 @@
         <v>1400.91</v>
       </c>
     </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A277" s="23">
         <v>45751</v>
       </c>
       <c r="F277">
         <v>712.75</v>
+      </c>
+      <c r="L277" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="278" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A278" s="23">
+        <v>45754</v>
+      </c>
+    </row>
+    <row r="279" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A279" s="23">
+        <v>45754</v>
+      </c>
+      <c r="F279" s="2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="280" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A280" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L280">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="281" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A281" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L281">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="282" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A282" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L282">
+        <v>431.25</v>
+      </c>
+    </row>
+    <row r="283" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A283" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L283">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="284" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A284" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L284">
+        <v>138.75</v>
+      </c>
+    </row>
+    <row r="285" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A285" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L285">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="286" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A286" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L286">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="287" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A287" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L287">
+        <v>543.75</v>
+      </c>
+    </row>
+    <row r="288" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A288" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L288">
+        <v>146.25</v>
+      </c>
+    </row>
+    <row r="289" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A289" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L289">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="290" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A290" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L290">
+        <v>337.5</v>
+      </c>
+    </row>
+    <row r="291" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A291" s="23">
+        <v>45754</v>
+      </c>
+      <c r="L291">
+        <v>131.25</v>
+      </c>
+    </row>
+    <row r="292" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A292" s="23">
+        <v>45754</v>
+      </c>
+      <c r="F292">
+        <v>1086.32</v>
+      </c>
+    </row>
+    <row r="293" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A293" s="23">
+        <v>45755</v>
+      </c>
+      <c r="L293">
+        <v>108.75</v>
+      </c>
+    </row>
+    <row r="294" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A294" s="23">
+        <v>45755</v>
+      </c>
+      <c r="F294">
+        <v>443.05</v>
+      </c>
+    </row>
+    <row r="295" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A295" s="23">
+        <v>45755</v>
+      </c>
+      <c r="L295">
+        <v>937.5</v>
+      </c>
+    </row>
+    <row r="296" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A296" s="23">
+        <v>45755</v>
+      </c>
+      <c r="L296">
+        <v>281.25</v>
+      </c>
+    </row>
+    <row r="297" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A297" s="23">
+        <v>45760</v>
+      </c>
+      <c r="L297">
+        <v>337.5</v>
+      </c>
+    </row>
+    <row r="298" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A298" s="23">
+        <v>45761</v>
+      </c>
+      <c r="L298">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="299" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A299" s="23">
+        <v>45762</v>
+      </c>
+      <c r="L299">
+        <v>281.25</v>
+      </c>
+    </row>
+    <row r="300" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A300" s="23">
+        <v>45763</v>
+      </c>
+      <c r="R300">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="301" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A301" s="23">
+        <v>45763</v>
+      </c>
+      <c r="R301">
+        <v>43.17</v>
+      </c>
+    </row>
+    <row r="302" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A302" s="23">
+        <v>45765</v>
+      </c>
+      <c r="R302">
+        <v>124.65</v>
+      </c>
+    </row>
+    <row r="303" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A303" s="23">
+        <v>45765</v>
+      </c>
+      <c r="R303">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="304" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A304" s="23">
+        <v>45768</v>
+      </c>
+      <c r="R304">
+        <v>66.790000000000006</v>
+      </c>
+    </row>
+    <row r="305" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A305" s="23">
+        <v>45768</v>
+      </c>
+      <c r="K305">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="306" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A306" s="23">
+        <v>45771</v>
+      </c>
+      <c r="R306">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="307" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A307" s="23">
+        <v>45771</v>
+      </c>
+      <c r="J307">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="308" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A308" s="23">
+        <v>45771</v>
+      </c>
+      <c r="M308">
+        <v>17.75</v>
+      </c>
+    </row>
+    <row r="309" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A309" s="23">
+        <v>45771</v>
+      </c>
+      <c r="N309" s="2">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="310" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A310" s="23">
+        <v>45771</v>
+      </c>
+      <c r="N310">
+        <v>264.14999999999998</v>
+      </c>
+    </row>
+    <row r="311" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A311" s="23">
+        <v>45772</v>
+      </c>
+      <c r="F311">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="312" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A312" s="23">
+        <v>45778</v>
+      </c>
+      <c r="M312">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="313" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A313" s="23">
+        <v>45786</v>
+      </c>
+      <c r="R313">
+        <v>41.42</v>
+      </c>
+    </row>
+    <row r="314" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A314" s="23">
+        <v>45786</v>
+      </c>
+      <c r="R314">
+        <v>122.1</v>
       </c>
     </row>
     <row r="349" spans="25:25" x14ac:dyDescent="0.35">
@@ -37793,7 +38842,7 @@
   <dimension ref="A1:V242"/>
   <sheetViews>
     <sheetView topLeftCell="A222" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A237" sqref="A237:XFD237"/>
+      <selection activeCell="B243" sqref="B243"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
@@ -40621,10 +41670,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8BED0-6F25-4951-9707-565F124E30A4}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -40729,6 +41778,27 @@
         <v>22778.539999999997</v>
       </c>
       <c r="G5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="23">
+        <v>45764</v>
+      </c>
+      <c r="B6" t="s">
+        <v>720</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1660</v>
+      </c>
+      <c r="E6">
+        <v>34.049999999999997</v>
+      </c>
+      <c r="F6" s="27">
+        <f>F5+E6-D6</f>
+        <v>22812.589999999997</v>
+      </c>
+      <c r="G6" t="s">
         <v>60</v>
       </c>
     </row>
@@ -40751,7 +41821,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEAEDB9-0FE6-48E6-8096-45942EADC73F}">
-  <dimension ref="A3:C24"/>
+  <dimension ref="A3:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -40759,9 +41829,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="2.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.59765625" bestFit="1" customWidth="1"/>
@@ -41006,7 +42076,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>240</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -41014,7 +42084,7 @@
         <v>89</v>
       </c>
       <c r="C7">
-        <v>245.4</v>
+        <v>480.01000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -41022,7 +42092,7 @@
         <v>113</v>
       </c>
       <c r="C8">
-        <v>97.6</v>
+        <v>121.07</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -41054,7 +42124,7 @@
         <v>983</v>
       </c>
       <c r="C12">
-        <v>210</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -41078,7 +42148,7 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>39.129999999999995</v>
+        <v>303.27999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -41102,7 +42172,7 @@
         <v>49</v>
       </c>
       <c r="C18">
-        <v>606.6</v>
+        <v>648.02</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -41137,7 +42207,7 @@
         <v>86</v>
       </c>
       <c r="B22">
-        <v>8167.81</v>
+        <v>8215.3100000000013</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -41145,18 +42215,34 @@
         <v>87</v>
       </c>
       <c r="C23">
-        <v>5426.25</v>
+        <v>5920.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24">
+        <v>1622.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C25">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B24">
-        <v>17501.960000000003</v>
-      </c>
-      <c r="C24">
-        <v>8721.09</v>
+      <c r="B26">
+        <v>17549.460000000003</v>
+      </c>
+      <c r="C26">
+        <v>13156.09</v>
       </c>
     </row>
   </sheetData>
@@ -41166,17 +42252,17 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FA1291-B9CE-4F7D-8600-2336ADED0E75}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
@@ -41200,87 +42286,111 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="26" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C4">
-        <v>25.4</v>
+        <v>1500</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>431.6</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="26" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7">
-        <v>8167.8099999999995</v>
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>431.6</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>5426.25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="26" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
       <c r="B9">
-        <v>2443.5300000000007</v>
+        <v>8215.31</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10">
-        <v>245.4</v>
+        <v>5920.5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="26" t="s">
-        <v>145</v>
+        <v>1</v>
       </c>
       <c r="B11">
-        <v>239.97</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
+        <v>2443.5300000000007</v>
       </c>
       <c r="E11" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12">
-        <v>10851.31</v>
+        <v>89</v>
       </c>
       <c r="C12">
-        <v>6358.65</v>
+        <v>480.01</v>
       </c>
       <c r="E12">
         <f>GETPIVOTDATA("Sum of Income",$A$3)-GETPIVOTDATA("Sum of Expenditure",$A$3)</f>
-        <v>4492.66</v>
+        <v>796.29999999999927</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="B13">
+        <v>239.97</v>
+      </c>
+      <c r="C13">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>170</v>
+      </c>
+      <c r="C14">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15">
+        <v>10898.81</v>
+      </c>
+      <c r="C15">
+        <v>10102.51</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -41288,7 +42398,7 @@
         <v>106</v>
       </c>
       <c r="B17" t="s">
-        <v>84</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -41321,10 +42431,10 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="26" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C20">
-        <v>132</v>
+        <v>122.1</v>
       </c>
       <c r="E20" t="s">
         <v>116</v>
@@ -41341,10 +42451,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21">
-        <v>30</v>
+        <v>49</v>
+      </c>
+      <c r="C21">
+        <v>41.42</v>
       </c>
       <c r="E21" t="s">
         <v>117</v>
@@ -41358,10 +42468,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="26" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C22">
-        <v>200</v>
+        <v>163.51999999999998</v>
       </c>
       <c r="E22" t="s">
         <v>97</v>
@@ -41373,102 +42483,6 @@
       <c r="H22">
         <f>SUM(H19:H21)</f>
         <v>8007.65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C23">
-        <v>30.49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="C24">
-        <v>613.22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27">
-        <v>39.129999999999995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="B29">
-        <v>1.77</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="26" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30">
-        <v>97.6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="26" t="s">
-        <v>180</v>
-      </c>
-      <c r="B31">
-        <v>6618.8800000000019</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="26" t="s">
-        <v>983</v>
-      </c>
-      <c r="C32">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="26" t="s">
-        <v>990</v>
-      </c>
-      <c r="C33">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="B34">
-        <v>6650.6500000000024</v>
-      </c>
-      <c r="C34">
-        <v>2362.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Young artists exhibition summary
</commit_message>
<xml_diff>
--- a/OAS 2025.xlsx
+++ b/OAS 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7D8860-274A-46F8-8EE5-A67428386689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E777978F-85B6-4968-9A6D-7C3B59DC240F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3533" yWindow="2228" windowWidth="16200" windowHeight="9307" firstSheet="1" activeTab="1" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" firstSheet="7" activeTab="8" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -29,15 +29,15 @@
     <sheet name="Lists" sheetId="9" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current account'!$A$1:$I$353</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Current account'!$A$1:$I$355</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Members Exhibition'!$A$1:$H$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Membership List'!$A$2:$A$216</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Stripe!$A$1:$W$478</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId15"/>
-    <pivotCache cacheId="10" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="1" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4662" uniqueCount="1749">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4709" uniqueCount="1766">
   <si>
     <t>Subs</t>
   </si>
@@ -5306,6 +5306,57 @@
   </si>
   <si>
     <t>Gifts to organisers</t>
+  </si>
+  <si>
+    <t>Phoebe Birch YA Prize</t>
+  </si>
+  <si>
+    <t>Ash Goller YA Prize</t>
+  </si>
+  <si>
+    <t>Amanda Jewell OAS</t>
+  </si>
+  <si>
+    <t>Drinks</t>
+  </si>
+  <si>
+    <t>Magdalen Road StudMAS hire</t>
+  </si>
+  <si>
+    <t>Meeting room hire</t>
+  </si>
+  <si>
+    <t>L Wootton-Davies OAS</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Erin 2</t>
+  </si>
+  <si>
+    <t>GROSS INTEREST TO 16JUN2025</t>
+  </si>
+  <si>
+    <t>Leaflet printing</t>
+  </si>
+  <si>
+    <t>Poster printing</t>
+  </si>
+  <si>
+    <t>Molly Palmer YA Prize</t>
+  </si>
+  <si>
+    <t>Flyers and  posters</t>
+  </si>
+  <si>
+    <t>Labels</t>
+  </si>
+  <si>
+    <t>Price list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost: </t>
   </si>
 </sst>
 </file>
@@ -5476,7 +5527,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -5524,7 +5575,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -5564,13 +5614,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45815.588818865741" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="331" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45827.539443634261" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="352" xr:uid="{52AA0CD4-A3EB-4892-953B-4445B6BC29AB}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I503" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-06-08T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-06-20T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5585,7 +5635,7 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="18411.630000000008"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5417.7200000000066" maxValue="18411.630000000008"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
       <sharedItems containsBlank="1" count="29">
@@ -5612,9 +5662,9 @@
         <s v="Exhibition organisers fees"/>
         <s v="Website manager's fee"/>
         <s v="Venue hire"/>
+        <s v="Admin"/>
         <s v="Exhibitions cr" u="1"/>
         <s v="Subs" u="1"/>
-        <s v="Admin" u="1"/>
         <s v="Prof Fees" u="1"/>
         <s v="Transfer Out" u="1"/>
         <s v="Honoraria" u="1"/>
@@ -5641,13 +5691,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45815.588925462966" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="331" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45827.539532407405" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="352" xr:uid="{B9AE540E-AB7F-4ADD-9804-695C06D03F39}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I400" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-06-08T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-06-20T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -5662,10 +5712,10 @@
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.77" maxValue="1690.92"/>
     </cacheField>
     <cacheField name="Balance" numFmtId="164">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5823.88" maxValue="18411.630000000008"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="5417.7200000000066" maxValue="18411.630000000008"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
-      <sharedItems containsBlank="1" count="24">
+      <sharedItems containsBlank="1" count="25">
         <m/>
         <s v="Subs 2025"/>
         <s v="Donations cr"/>
@@ -5689,6 +5739,7 @@
         <s v="Exhibition organisers fees"/>
         <s v="Website manager's fee"/>
         <s v="Venue hire"/>
+        <s v="Admin"/>
         <s v="Exhibitions cr" u="1"/>
       </sharedItems>
     </cacheField>
@@ -5708,7 +5759,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="331">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="352">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -8270,7 +8321,7 @@
     <n v="10805.810000000005"/>
     <x v="14"/>
     <x v="1"/>
-    <m/>
+    <s v="Flyers and  posters"/>
   </r>
   <r>
     <d v="2025-02-26T00:00:00"/>
@@ -8598,9 +8649,9 @@
     <n v="63.6"/>
     <m/>
     <n v="11761.400000000007"/>
-    <x v="14"/>
-    <x v="1"/>
-    <m/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="Labels"/>
   </r>
   <r>
     <d v="2025-03-24T00:00:00"/>
@@ -8611,7 +8662,7 @@
     <n v="11624.400000000007"/>
     <x v="14"/>
     <x v="1"/>
-    <m/>
+    <s v="Price list"/>
   </r>
   <r>
     <d v="2025-03-24T00:00:00"/>
@@ -9150,7 +9201,7 @@
     <n v="10339.350000000008"/>
     <x v="14"/>
     <x v="2"/>
-    <m/>
+    <s v="Leaflet printing"/>
   </r>
   <r>
     <d v="2025-05-09T00:00:00"/>
@@ -9293,7 +9344,7 @@
     <n v="7435.2000000000071"/>
     <x v="14"/>
     <x v="2"/>
-    <m/>
+    <s v="Poster printing"/>
   </r>
   <r>
     <d v="2025-06-06T00:00:00"/>
@@ -9340,6 +9391,237 @@
     <s v="Gifts to organisers"/>
   </r>
   <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Phoebe Birch YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="7279.7000000000071"/>
+    <x v="16"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Ash Goller YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="7179.7000000000071"/>
+    <x v="16"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Amanda Jewell OAS"/>
+    <n v="220.68"/>
+    <m/>
+    <n v="6959.0200000000068"/>
+    <x v="4"/>
+    <x v="2"/>
+    <s v="Drinks"/>
+  </r>
+  <r>
+    <d v="2025-06-13T00:00:00"/>
+    <s v="BP"/>
+    <s v="Magdalen Road StudMAS hire"/>
+    <n v="225"/>
+    <m/>
+    <n v="6734.0200000000068"/>
+    <x v="23"/>
+    <x v="0"/>
+    <s v="Meeting room hire"/>
+  </r>
+  <r>
+    <d v="2025-06-13T00:00:00"/>
+    <s v="BP"/>
+    <s v="Magdalen Road StudMAS hire"/>
+    <n v="700"/>
+    <m/>
+    <n v="6034.0200000000068"/>
+    <x v="22"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="L Wootton-Davies OAS"/>
+    <n v="319.2"/>
+    <m/>
+    <n v="5714.820000000007"/>
+    <x v="20"/>
+    <x v="2"/>
+    <s v="Louis"/>
+  </r>
+  <r>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="197.1"/>
+    <m/>
+    <n v="5517.7200000000066"/>
+    <x v="20"/>
+    <x v="2"/>
+    <s v="Erin 2"/>
+  </r>
+  <r>
+    <d v="2025-06-19T00:00:00"/>
+    <s v="BP"/>
+    <s v="Molly Palmer YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="5417.7200000000066"/>
+    <x v="16"/>
+    <x v="2"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -9354,7 +9636,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="331">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="352">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -11916,7 +12198,7 @@
     <n v="10805.810000000005"/>
     <x v="14"/>
     <s v="Members"/>
-    <m/>
+    <s v="Flyers and  posters"/>
   </r>
   <r>
     <d v="2025-02-26T00:00:00"/>
@@ -12244,9 +12526,9 @@
     <n v="63.6"/>
     <m/>
     <n v="11761.400000000007"/>
-    <x v="14"/>
+    <x v="4"/>
     <s v="Members"/>
-    <m/>
+    <s v="Labels"/>
   </r>
   <r>
     <d v="2025-03-24T00:00:00"/>
@@ -12257,7 +12539,7 @@
     <n v="11624.400000000007"/>
     <x v="14"/>
     <s v="Members"/>
-    <m/>
+    <s v="Price list"/>
   </r>
   <r>
     <d v="2025-03-24T00:00:00"/>
@@ -12796,7 +13078,7 @@
     <n v="10339.350000000008"/>
     <x v="14"/>
     <s v="Young artists"/>
-    <m/>
+    <s v="Leaflet printing"/>
   </r>
   <r>
     <d v="2025-05-09T00:00:00"/>
@@ -12939,7 +13221,7 @@
     <n v="7435.2000000000071"/>
     <x v="14"/>
     <s v="Young artists"/>
-    <m/>
+    <s v="Poster printing"/>
   </r>
   <r>
     <d v="2025-06-06T00:00:00"/>
@@ -12986,6 +13268,237 @@
     <s v="Gifts to organisers"/>
   </r>
   <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Phoebe Birch YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="7279.7000000000071"/>
+    <x v="16"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Ash Goller YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="7179.7000000000071"/>
+    <x v="16"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-10T00:00:00"/>
+    <s v="BP"/>
+    <s v="Amanda Jewell OAS"/>
+    <n v="220.68"/>
+    <m/>
+    <n v="6959.0200000000068"/>
+    <x v="4"/>
+    <s v="Young artists"/>
+    <s v="Drinks"/>
+  </r>
+  <r>
+    <d v="2025-06-13T00:00:00"/>
+    <s v="BP"/>
+    <s v="Magdalen Road StudMAS hire"/>
+    <n v="225"/>
+    <m/>
+    <n v="6734.0200000000068"/>
+    <x v="23"/>
+    <m/>
+    <s v="Meeting room hire"/>
+  </r>
+  <r>
+    <d v="2025-06-13T00:00:00"/>
+    <s v="BP"/>
+    <s v="Magdalen Road StudMAS hire"/>
+    <n v="700"/>
+    <m/>
+    <n v="6034.0200000000068"/>
+    <x v="22"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="L Wootton-Davies OAS"/>
+    <n v="319.2"/>
+    <m/>
+    <n v="5714.820000000007"/>
+    <x v="20"/>
+    <s v="Young artists"/>
+    <s v="Louis"/>
+  </r>
+  <r>
+    <d v="2025-06-16T00:00:00"/>
+    <s v="BP"/>
+    <s v="Erin Thomas OAS"/>
+    <n v="197.1"/>
+    <m/>
+    <n v="5517.7200000000066"/>
+    <x v="20"/>
+    <s v="Young artists"/>
+    <s v="Erin 2"/>
+  </r>
+  <r>
+    <d v="2025-06-19T00:00:00"/>
+    <s v="BP"/>
+    <s v="Molly Palmer YA Prize"/>
+    <n v="100"/>
+    <m/>
+    <n v="5417.7200000000066"/>
+    <x v="16"/>
+    <s v="Young artists"/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -13000,8 +13513,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB64E1A4-8455-499E-80FF-BC0BFCCF7279}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C27" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EB64E1A4-8455-499E-80FF-BC0BFCCF7279}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C28" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -13010,7 +13523,7 @@
     <pivotField dataField="1" showAll="0"/>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
-      <items count="25">
+      <items count="26">
         <item x="1"/>
         <item x="0"/>
         <item x="3"/>
@@ -13029,12 +13542,13 @@
         <item x="15"/>
         <item x="16"/>
         <item x="17"/>
-        <item m="1" x="23"/>
+        <item m="1" x="24"/>
         <item x="18"/>
         <item x="19"/>
         <item x="20"/>
         <item x="21"/>
         <item x="22"/>
+        <item x="23"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -13044,7 +13558,7 @@
   <rowFields count="1">
     <field x="6"/>
   </rowFields>
-  <rowItems count="24">
+  <rowItems count="25">
     <i>
       <x/>
     </i>
@@ -13114,6 +13628,9 @@
     <i>
       <x v="23"/>
     </i>
+    <i>
+      <x v="24"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -13146,8 +13663,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:C16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A22:C31" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
     <pivotField showAll="0"/>
@@ -13157,7 +13674,7 @@
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="30">
-        <item m="1" x="25"/>
+        <item x="23"/>
         <item x="7"/>
         <item x="2"/>
         <item x="6"/>
@@ -13171,7 +13688,7 @@
         <item x="18"/>
         <item x="19"/>
         <item x="13"/>
-        <item m="1" x="24"/>
+        <item m="1" x="25"/>
         <item x="11"/>
         <item x="22"/>
         <item x="0"/>
@@ -13185,7 +13702,124 @@
         <item x="1"/>
         <item x="8"/>
         <item x="10"/>
-        <item m="1" x="23"/>
+        <item m="1" x="24"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="7" item="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:C16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="15" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="30">
+        <item x="23"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="20"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item m="1" x="26"/>
+        <item x="14"/>
+        <item x="3"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item m="1" x="25"/>
+        <item x="11"/>
+        <item x="22"/>
+        <item x="0"/>
+        <item x="12"/>
+        <item x="4"/>
+        <item m="1" x="28"/>
+        <item x="5"/>
+        <item x="15"/>
+        <item m="1" x="27"/>
+        <item x="21"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item m="1" x="24"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -13257,117 +13891,6 @@
   </colItems>
   <pageFields count="1">
     <pageField fld="7" item="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A22:C29" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="9">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="30">
-        <item m="1" x="25"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="20"/>
-        <item x="9"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item m="1" x="26"/>
-        <item x="14"/>
-        <item x="3"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="13"/>
-        <item m="1" x="24"/>
-        <item x="11"/>
-        <item x="22"/>
-        <item x="0"/>
-        <item x="12"/>
-        <item x="4"/>
-        <item m="1" x="28"/>
-        <item x="5"/>
-        <item x="15"/>
-        <item m="1" x="27"/>
-        <item x="21"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item m="1" x="23"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="7">
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="7" item="3" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
@@ -13691,22 +14214,22 @@
   <sheetFormatPr defaultColWidth="8.19921875" defaultRowHeight="13.15" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.796875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" style="5" customWidth="1"/>
+    <col min="2" max="2" width="14.1328125" style="5" customWidth="1"/>
     <col min="3" max="3" width="11.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.19921875" style="5"/>
-    <col min="5" max="5" width="16.53125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="16.59765625" style="5" customWidth="1"/>
     <col min="6" max="6" width="11.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="8.19921875" style="5"/>
     <col min="9" max="9" width="24.796875" style="5" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="5" customWidth="1"/>
     <col min="11" max="11" width="11.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.19921875" style="5"/>
-    <col min="13" max="13" width="22.33203125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="22.3984375" style="5" customWidth="1"/>
     <col min="14" max="14" width="8.19921875" style="5"/>
     <col min="15" max="15" width="11.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="18" width="8.19921875" style="5"/>
-    <col min="19" max="19" width="9.19921875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.53125" style="5" customWidth="1"/>
+    <col min="19" max="19" width="9.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.59765625" style="5" customWidth="1"/>
     <col min="21" max="16384" width="8.19921875" style="5"/>
   </cols>
   <sheetData>
@@ -13905,7 +14428,7 @@
       <c r="J7" s="17"/>
       <c r="K7" s="31">
         <f>SUMIF('Savings account'!G2:G15, "Interest", 'Savings account'!E2:E15)</f>
-        <v>167.39000000000001</v>
+        <v>199.21</v>
       </c>
       <c r="L7" s="17"/>
       <c r="M7" s="17" t="s">
@@ -13914,7 +14437,7 @@
       <c r="N7" s="17"/>
       <c r="O7" s="31">
         <f>SUMIF('Current account'!G2:G401,"Admin",'Current account'!D2:D401)+SUMIF('Current account'!G2:G401, "Other expenses", 'Current account'!D2:D401)</f>
-        <v>126.07</v>
+        <v>351.07</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.4">
@@ -13957,7 +14480,7 @@
       </c>
       <c r="F9" s="31">
         <f>GETPIVOTDATA("Sum of Expenditure",Exhibitions!$A$3,"Category","Publicity")</f>
-        <v>431.6</v>
+        <v>368</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -14051,7 +14574,7 @@
       <c r="E12" s="17"/>
       <c r="F12" s="31">
         <f>SUM(F5:F11)</f>
-        <v>5598.71</v>
+        <v>5535.11</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -14126,7 +14649,7 @@
       <c r="N15" s="17"/>
       <c r="O15" s="31">
         <f ca="1">SUM(O4:O13)</f>
-        <v>2537.46</v>
+        <v>2762.46</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.45">
@@ -19757,16 +20280,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.06640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.19921875" customWidth="1"/>
     <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.59765625" customWidth="1"/>
-    <col min="11" max="11" width="68.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.53125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.46484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.9296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="53.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="53.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
@@ -28949,18 +29472,18 @@
   <cols>
     <col min="1" max="1" width="16.46484375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="5"/>
-    <col min="3" max="3" width="26.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1328125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.06640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.9296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="5"/>
-    <col min="10" max="10" width="17.33203125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="17.3984375" style="5" customWidth="1"/>
     <col min="11" max="11" width="35.19921875" style="5" customWidth="1"/>
     <col min="12" max="12" width="9" style="5" customWidth="1"/>
     <col min="13" max="13" width="22" style="5" customWidth="1"/>
-    <col min="14" max="14" width="7.46484375" style="5" customWidth="1"/>
-    <col min="15" max="15" width="9.265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.3984375" style="5" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.53125" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.796875" style="5" customWidth="1"/>
     <col min="18" max="18" width="10.53125" style="5" bestFit="1" customWidth="1"/>
@@ -29937,10 +30460,10 @@
     <col min="6" max="7" width="9" style="5"/>
     <col min="8" max="8" width="6.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21" style="5" customWidth="1"/>
-    <col min="10" max="10" width="13.9296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.86328125" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="26" width="9" style="5"/>
     <col min="27" max="27" width="25.19921875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="32.73046875" style="5" customWidth="1"/>
+    <col min="28" max="28" width="32.796875" style="5" customWidth="1"/>
     <col min="29" max="29" width="9" style="9"/>
     <col min="30" max="30" width="9" style="5"/>
     <col min="31" max="32" width="15.53125" style="5" customWidth="1"/>
@@ -29985,7 +30508,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.15" x14ac:dyDescent="0.4">
@@ -30163,20 +30686,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I331"/>
+  <dimension ref="A1:I339"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A315" workbookViewId="0">
-      <selection activeCell="I332" sqref="I332"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G361" sqref="G361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.19921875" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.35">
@@ -34888,7 +35411,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225" s="23">
         <v>45706</v>
       </c>
@@ -34912,7 +35435,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226" s="23">
         <v>45707</v>
       </c>
@@ -34936,7 +35459,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227" s="23">
         <v>45707</v>
       </c>
@@ -34957,7 +35480,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228" s="23">
         <v>45707</v>
       </c>
@@ -34978,7 +35501,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229" s="23">
         <v>45708</v>
       </c>
@@ -35002,7 +35525,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230" s="23">
         <v>45709</v>
       </c>
@@ -35026,7 +35549,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231" s="23">
         <v>45709</v>
       </c>
@@ -35047,7 +35570,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232" s="23">
         <v>45712</v>
       </c>
@@ -35071,7 +35594,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233" s="23">
         <v>45713</v>
       </c>
@@ -35095,7 +35618,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234" s="23">
         <v>45713</v>
       </c>
@@ -35118,8 +35641,11 @@
       <c r="H234" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I234" t="s">
+        <v>1762</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235" s="23">
         <v>45714</v>
       </c>
@@ -35140,7 +35666,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236" s="23">
         <v>45714</v>
       </c>
@@ -35164,7 +35690,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237" s="23">
         <v>45715</v>
       </c>
@@ -35188,7 +35714,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238" s="23">
         <v>45716</v>
       </c>
@@ -35212,7 +35738,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239" s="23">
         <v>45719</v>
       </c>
@@ -35236,7 +35762,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240" s="23">
         <v>45719</v>
       </c>
@@ -35803,10 +36329,13 @@
         <v>11761.400000000007</v>
       </c>
       <c r="G264" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="H264" t="s">
         <v>104</v>
+      </c>
+      <c r="I264" t="s">
+        <v>1763</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.35">
@@ -35832,6 +36361,9 @@
       <c r="H265" t="s">
         <v>104</v>
       </c>
+      <c r="I265" t="s">
+        <v>1764</v>
+      </c>
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266" s="23">
@@ -35943,7 +36475,7 @@
         <v>80.599999999999994</v>
       </c>
       <c r="F270" s="24">
-        <f t="shared" ref="F270:F331" si="5">F269+E270-D270</f>
+        <f t="shared" ref="F270:F335" si="5">F269+E270-D270</f>
         <v>14864.150000000009</v>
       </c>
       <c r="G270" t="s">
@@ -36996,6 +37528,9 @@
       <c r="H314" t="s">
         <v>1668</v>
       </c>
+      <c r="I314" t="s">
+        <v>1759</v>
+      </c>
     </row>
     <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315" s="23">
@@ -37305,6 +37840,9 @@
       <c r="H327" t="s">
         <v>1668</v>
       </c>
+      <c r="I327" t="s">
+        <v>1760</v>
+      </c>
     </row>
     <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328" s="23">
@@ -37408,8 +37946,209 @@
         <v>1748</v>
       </c>
     </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A332" s="23">
+        <v>45818</v>
+      </c>
+      <c r="B332" t="s">
+        <v>264</v>
+      </c>
+      <c r="C332" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D332">
+        <v>100</v>
+      </c>
+      <c r="F332" s="24">
+        <f t="shared" si="5"/>
+        <v>7279.7000000000071</v>
+      </c>
+      <c r="G332" t="s">
+        <v>10</v>
+      </c>
+      <c r="H332" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A333" s="23">
+        <v>45818</v>
+      </c>
+      <c r="B333" t="s">
+        <v>264</v>
+      </c>
+      <c r="C333" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D333">
+        <v>100</v>
+      </c>
+      <c r="F333" s="24">
+        <f t="shared" si="5"/>
+        <v>7179.7000000000071</v>
+      </c>
+      <c r="G333" t="s">
+        <v>10</v>
+      </c>
+      <c r="H333" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A334" s="23">
+        <v>45818</v>
+      </c>
+      <c r="B334" t="s">
+        <v>264</v>
+      </c>
+      <c r="C334" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D334">
+        <v>220.68</v>
+      </c>
+      <c r="F334" s="24">
+        <f t="shared" si="5"/>
+        <v>6959.0200000000068</v>
+      </c>
+      <c r="G334" t="s">
+        <v>89</v>
+      </c>
+      <c r="H334" t="s">
+        <v>1668</v>
+      </c>
+      <c r="I334" t="s">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A335" s="23">
+        <v>45821</v>
+      </c>
+      <c r="B335" t="s">
+        <v>264</v>
+      </c>
+      <c r="C335" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D335">
+        <v>225</v>
+      </c>
+      <c r="F335" s="24">
+        <f t="shared" si="5"/>
+        <v>6734.0200000000068</v>
+      </c>
+      <c r="G335" t="s">
+        <v>6</v>
+      </c>
+      <c r="I335" t="s">
+        <v>1754</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A336" s="23">
+        <v>45821</v>
+      </c>
+      <c r="B336" t="s">
+        <v>264</v>
+      </c>
+      <c r="C336" t="s">
+        <v>1753</v>
+      </c>
+      <c r="D336">
+        <v>700</v>
+      </c>
+      <c r="F336" s="24">
+        <f t="shared" ref="F336:F339" si="6">F335+E336-D336</f>
+        <v>6034.0200000000068</v>
+      </c>
+      <c r="G336" t="s">
+        <v>102</v>
+      </c>
+      <c r="H336" t="s">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A337" s="23">
+        <v>45824</v>
+      </c>
+      <c r="B337" t="s">
+        <v>264</v>
+      </c>
+      <c r="C337" t="s">
+        <v>1755</v>
+      </c>
+      <c r="D337">
+        <v>319.2</v>
+      </c>
+      <c r="F337" s="24">
+        <f t="shared" si="6"/>
+        <v>5714.820000000007</v>
+      </c>
+      <c r="G337" t="s">
+        <v>103</v>
+      </c>
+      <c r="H337" t="s">
+        <v>1668</v>
+      </c>
+      <c r="I337" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A338" s="23">
+        <v>45824</v>
+      </c>
+      <c r="B338" t="s">
+        <v>264</v>
+      </c>
+      <c r="C338" t="s">
+        <v>1667</v>
+      </c>
+      <c r="D338">
+        <v>197.1</v>
+      </c>
+      <c r="F338" s="24">
+        <f t="shared" si="6"/>
+        <v>5517.7200000000066</v>
+      </c>
+      <c r="G338" t="s">
+        <v>103</v>
+      </c>
+      <c r="H338" t="s">
+        <v>1668</v>
+      </c>
+      <c r="I338" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A339" s="23">
+        <v>45827</v>
+      </c>
+      <c r="B339" t="s">
+        <v>264</v>
+      </c>
+      <c r="C339" t="s">
+        <v>1761</v>
+      </c>
+      <c r="D339">
+        <v>100</v>
+      </c>
+      <c r="F339" s="24">
+        <f t="shared" si="6"/>
+        <v>5417.7200000000066</v>
+      </c>
+      <c r="G339" t="s">
+        <v>10</v>
+      </c>
+      <c r="H339" t="s">
+        <v>1668</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I353" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
+  <autoFilter ref="A1:I355" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -37449,7 +38188,7 @@
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.59765625" customWidth="1"/>
     <col min="3" max="3" width="18.19921875" customWidth="1"/>
-    <col min="4" max="20" width="12.59765625" style="2" customWidth="1"/>
+    <col min="4" max="20" width="12.53125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
@@ -40649,12 +41388,12 @@
   <cols>
     <col min="1" max="1" width="11.59765625" style="5" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.73046875" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="10.06640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="10.1328125" style="5" customWidth="1"/>
     <col min="4" max="5" width="8.19921875" style="5"/>
     <col min="6" max="6" width="11.06640625" style="5" customWidth="1"/>
     <col min="7" max="7" width="8.19921875" style="5"/>
-    <col min="8" max="8" width="10.59765625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="9.19921875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.19921875" style="5"/>
   </cols>
   <sheetData>
@@ -40785,9 +41524,9 @@
   <cols>
     <col min="1" max="1" width="42.19921875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.265625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.53125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="13" width="9" style="5"/>
-    <col min="14" max="15" width="18.9296875" style="5" customWidth="1"/>
+    <col min="14" max="15" width="18.86328125" style="5" customWidth="1"/>
     <col min="16" max="18" width="9" style="5"/>
     <col min="19" max="20" width="32.19921875" style="5" customWidth="1"/>
     <col min="21" max="21" width="18.46484375" style="5" customWidth="1"/>
@@ -40795,7 +41534,7 @@
     <col min="23" max="23" width="11.06640625" style="5" customWidth="1"/>
     <col min="24" max="24" width="9" style="5"/>
     <col min="25" max="25" width="10.53125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.46484375" style="5" customWidth="1"/>
+    <col min="26" max="26" width="14.3984375" style="5" customWidth="1"/>
     <col min="27" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
@@ -43522,7 +44261,7 @@
     <col min="1" max="1" width="8.73046875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.06640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="8.19921875" style="5"/>
-    <col min="15" max="15" width="24.06640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="8.19921875" style="5"/>
   </cols>
   <sheetData>
@@ -43606,17 +44345,17 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8BED0-6F25-4951-9707-565F124E30A4}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.06640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.19921875" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -43668,7 +44407,7 @@
         <v>36.21</v>
       </c>
       <c r="F3" s="27">
-        <f>F2+E3-D3</f>
+        <f t="shared" ref="F3:F8" si="0">F2+E3-D3</f>
         <v>22713.059999999998</v>
       </c>
       <c r="G3" t="s">
@@ -43689,7 +44428,7 @@
         <v>34.770000000000003</v>
       </c>
       <c r="F4" s="27">
-        <f>F3+E4-D4</f>
+        <f t="shared" si="0"/>
         <v>22747.829999999998</v>
       </c>
       <c r="G4" t="s">
@@ -43710,7 +44449,7 @@
         <v>30.71</v>
       </c>
       <c r="F5" s="27">
-        <f>F4+E5-D5</f>
+        <f t="shared" si="0"/>
         <v>22778.539999999997</v>
       </c>
       <c r="G5" t="s">
@@ -43731,7 +44470,7 @@
         <v>34.049999999999997</v>
       </c>
       <c r="F6" s="27">
-        <f>F5+E6-D6</f>
+        <f t="shared" si="0"/>
         <v>22812.589999999997</v>
       </c>
       <c r="G6" t="s">
@@ -43752,10 +44491,31 @@
         <v>31.65</v>
       </c>
       <c r="F7" s="27">
-        <f>F6+E7-D7</f>
+        <f t="shared" si="0"/>
         <v>22844.239999999998</v>
       </c>
       <c r="G7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="23">
+        <v>45825</v>
+      </c>
+      <c r="B8" t="s">
+        <v>720</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E8">
+        <v>31.82</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="0"/>
+        <v>22876.059999999998</v>
+      </c>
+      <c r="G8" t="s">
         <v>60</v>
       </c>
     </row>
@@ -43778,7 +44538,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEAEDB9-0FE6-48E6-8096-45942EADC73F}">
-  <dimension ref="A3:C27"/>
+  <dimension ref="A3:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
@@ -43813,12 +44573,12 @@
     <col min="36" max="36" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="15" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.9296875" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="43" max="45" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="43" max="45" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="6.9296875" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="6.86328125" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="6.73046875" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="11.06640625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="15" bestFit="1" customWidth="1"/>
@@ -43869,31 +44629,31 @@
     <col min="97" max="97" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="15" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="20" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="19.9296875" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="15" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="15" bestFit="1" customWidth="1"/>
     <col min="107" max="107" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="109" max="109" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="110" max="110" width="15" bestFit="1" customWidth="1"/>
     <col min="111" max="111" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="113" max="113" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="114" max="114" width="15" bestFit="1" customWidth="1"/>
     <col min="115" max="115" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="117" max="117" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="118" max="118" width="15" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="122" max="122" width="15" bestFit="1" customWidth="1"/>
     <col min="123" max="123" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="124" max="124" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="125" max="125" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="126" max="126" width="15" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -43901,35 +44661,35 @@
     <col min="129" max="129" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="130" max="130" width="15" bestFit="1" customWidth="1"/>
     <col min="131" max="131" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="133" max="133" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="134" max="134" width="15" bestFit="1" customWidth="1"/>
     <col min="135" max="135" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="137" max="137" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="138" max="138" width="15" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="141" max="141" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="142" max="142" width="15" bestFit="1" customWidth="1"/>
     <col min="143" max="143" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="145" max="145" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="146" max="146" width="15" bestFit="1" customWidth="1"/>
     <col min="147" max="147" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="148" max="148" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="148" max="148" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="149" max="149" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="150" max="150" width="15" bestFit="1" customWidth="1"/>
     <col min="151" max="151" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="153" max="153" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="154" max="154" width="15" bestFit="1" customWidth="1"/>
     <col min="155" max="155" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="157" max="157" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="158" max="158" width="15" bestFit="1" customWidth="1"/>
     <col min="159" max="159" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="161" max="161" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="162" max="162" width="15" bestFit="1" customWidth="1"/>
     <col min="163" max="163" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -43937,15 +44697,15 @@
     <col min="165" max="165" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="166" max="166" width="15" bestFit="1" customWidth="1"/>
     <col min="167" max="167" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="169" max="169" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="170" max="170" width="15" bestFit="1" customWidth="1"/>
     <col min="171" max="171" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="172" max="172" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="172" max="172" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="173" max="173" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="174" max="174" width="15" bestFit="1" customWidth="1"/>
     <col min="175" max="175" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="177" max="177" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="178" max="178" width="15" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -43953,15 +44713,15 @@
     <col min="181" max="181" width="18.46484375" bestFit="1" customWidth="1"/>
     <col min="182" max="182" width="15" bestFit="1" customWidth="1"/>
     <col min="183" max="183" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="185" max="185" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="186" max="186" width="15" bestFit="1" customWidth="1"/>
     <col min="187" max="187" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="189" max="189" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="190" max="190" width="15" bestFit="1" customWidth="1"/>
     <col min="191" max="191" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="21.265625" bestFit="1" customWidth="1"/>
+    <col min="192" max="192" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="193" max="193" width="19.53125" bestFit="1" customWidth="1"/>
     <col min="194" max="194" width="15" bestFit="1" customWidth="1"/>
     <col min="195" max="195" width="13.33203125" bestFit="1" customWidth="1"/>
@@ -43999,8 +44759,8 @@
     <col min="227" max="227" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="228" max="228" width="15" bestFit="1" customWidth="1"/>
     <col min="229" max="229" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="21.53125" bestFit="1" customWidth="1"/>
-    <col min="231" max="232" width="20" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="231" max="232" width="19.9296875" bestFit="1" customWidth="1"/>
     <col min="233" max="233" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -44019,24 +44779,20 @@
       <c r="A4" s="26" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="43">
+      <c r="B4">
         <v>6618.8800000000019</v>
       </c>
-      <c r="C4" s="43"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43">
+      <c r="C6">
         <v>255</v>
       </c>
     </row>
@@ -44044,17 +44800,15 @@
       <c r="A7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43">
-        <v>495.51000000000005</v>
+      <c r="C7">
+        <v>779.79</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43">
+      <c r="C8">
         <v>126.07</v>
       </c>
     </row>
@@ -44062,17 +44816,15 @@
       <c r="A9" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9">
         <v>230</v>
       </c>
-      <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43">
+      <c r="C10">
         <v>200</v>
       </c>
     </row>
@@ -44080,8 +44832,7 @@
       <c r="A11" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43">
+      <c r="C11">
         <v>132</v>
       </c>
     </row>
@@ -44089,8 +44840,7 @@
       <c r="A12" s="26" t="s">
         <v>983</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43">
+      <c r="C12">
         <v>450</v>
       </c>
     </row>
@@ -44098,8 +44848,7 @@
       <c r="A13" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43">
+      <c r="C13">
         <v>105.89</v>
       </c>
     </row>
@@ -44107,8 +44856,7 @@
       <c r="A14" s="26" t="s">
         <v>990</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43">
+      <c r="C14">
         <v>812.5</v>
       </c>
     </row>
@@ -44116,8 +44864,7 @@
       <c r="A15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43">
+      <c r="C15">
         <v>1360.28</v>
       </c>
     </row>
@@ -44125,37 +44872,34 @@
       <c r="A16" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16">
         <v>1.77</v>
       </c>
-      <c r="C16" s="43"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="43">
+      <c r="B17">
         <v>2700.95</v>
       </c>
-      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43">
-        <v>675.88</v>
+      <c r="C18">
+        <v>612.28</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="43">
+      <c r="B19">
         <v>239.97</v>
       </c>
-      <c r="C19" s="43">
+      <c r="C19">
         <v>30</v>
       </c>
     </row>
@@ -44163,17 +44907,15 @@
       <c r="A20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43">
-        <v>200</v>
+      <c r="C20">
+        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43">
+      <c r="C21">
         <v>613.22</v>
       </c>
     </row>
@@ -44181,17 +44923,15 @@
       <c r="A22" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="43">
+      <c r="B22">
         <v>8215.3100000000013</v>
       </c>
-      <c r="C22" s="43"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43">
+      <c r="C23">
         <v>5920.5</v>
       </c>
     </row>
@@ -44199,17 +44939,15 @@
       <c r="A24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43">
-        <v>1622.1</v>
+      <c r="C24">
+        <v>2138.4</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43">
+      <c r="C25">
         <v>1500</v>
       </c>
     </row>
@@ -44217,20 +44955,27 @@
       <c r="A26" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43">
-        <v>1952.11</v>
+      <c r="C26">
+        <v>2652.1099999999997</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B28">
         <v>18006.880000000005</v>
       </c>
-      <c r="C27" s="43">
-        <v>16451.060000000001</v>
+      <c r="C28">
+        <v>18413.039999999997</v>
       </c>
     </row>
   </sheetData>
@@ -44240,10 +44985,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60FA1291-B9CE-4F7D-8600-2336ADED0E75}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -44276,8 +45021,7 @@
       <c r="A4" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43">
+      <c r="C4">
         <v>1500</v>
       </c>
       <c r="E4" t="s">
@@ -44288,8 +45032,7 @@
       <c r="A5" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43">
+      <c r="C5">
         <v>25.4</v>
       </c>
       <c r="E5" t="s">
@@ -44309,8 +45052,7 @@
       <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43">
+      <c r="C6">
         <v>200</v>
       </c>
       <c r="E6" t="s">
@@ -44330,9 +45072,8 @@
       <c r="A7" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43">
-        <v>431.6</v>
+      <c r="C7">
+        <v>368</v>
       </c>
       <c r="E7" t="s">
         <v>117</v>
@@ -44348,8 +45089,7 @@
       <c r="A8" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43">
+      <c r="C8">
         <v>15</v>
       </c>
       <c r="E8" t="s">
@@ -44368,17 +45108,15 @@
       <c r="A9" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B9" s="43">
+      <c r="B9">
         <v>8215.31</v>
       </c>
-      <c r="C9" s="43"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43">
+      <c r="C10">
         <v>5920.5</v>
       </c>
     </row>
@@ -44386,10 +45124,9 @@
       <c r="A11" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="43">
+      <c r="B11">
         <v>2443.5300000000007</v>
       </c>
-      <c r="C11" s="43"/>
       <c r="E11" t="s">
         <v>1646</v>
       </c>
@@ -44405,8 +45142,7 @@
       <c r="A12" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43">
+      <c r="C12">
         <v>1952.11</v>
       </c>
       <c r="E12">
@@ -44418,19 +45154,18 @@
       <c r="A13" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43">
-        <v>480.01</v>
+      <c r="C13">
+        <v>543.61</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="43">
+      <c r="B14">
         <v>239.97</v>
       </c>
-      <c r="C14" s="43">
+      <c r="C14">
         <v>30</v>
       </c>
     </row>
@@ -44438,8 +45173,7 @@
       <c r="A15" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43">
+      <c r="C15">
         <v>1500</v>
       </c>
     </row>
@@ -44447,14 +45181,14 @@
       <c r="A16" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="43">
+      <c r="B16">
         <v>10898.81</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16">
         <v>12054.62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="25" t="s">
         <v>106</v>
       </c>
@@ -44462,7 +45196,7 @@
         <v>1668</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="25" t="s">
         <v>82</v>
       </c>
@@ -44473,69 +45207,86 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23">
         <v>200</v>
       </c>
-      <c r="C23" s="43"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43">
-        <v>122.1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>638.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="43">
+      <c r="C25">
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43">
+      <c r="C27">
         <v>69.28</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="26" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B28">
         <v>257.41999999999996</v>
       </c>
-      <c r="C27" s="43"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="26" t="s">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="26" t="s">
+      <c r="C30">
+        <v>236.18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B31">
         <v>457.41999999999996</v>
       </c>
-      <c r="C29" s="43">
-        <v>256.88</v>
+      <c r="C31">
+        <v>1993.8600000000001</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F31">
+        <f>GETPIVOTDATA("Sum of Expenditure",$A$22)-GETPIVOTDATA("Sum of Income",$A$22)</f>
+        <v>1536.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update previous year calculation to be consistent with current year
</commit_message>
<xml_diff>
--- a/OAS 2025.xlsx
+++ b/OAS 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\OAS_Finances_2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F9A767C-DB06-41C1-A77A-B421C3223D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45ED0A85-3611-4F5E-920F-4E3948699060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="16199" windowHeight="9847" firstSheet="4" activeTab="6" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" activeTab="1" xr2:uid="{E6A7689A-682B-425D-92A3-B87F804748A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="17" r:id="rId1"/>
@@ -36,8 +36,8 @@
   </definedNames>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId15"/>
-    <pivotCache cacheId="3" r:id="rId16"/>
+    <pivotCache cacheId="0" r:id="rId15"/>
+    <pivotCache cacheId="9" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6600" uniqueCount="2321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6607" uniqueCount="2322">
   <si>
     <t>Subs</t>
   </si>
@@ -7022,6 +7022,9 @@
   </si>
   <si>
     <t>Invoice 1027617, poster encapsulation</t>
+  </si>
+  <si>
+    <t>Domain name</t>
   </si>
 </sst>
 </file>
@@ -7206,7 +7209,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -7261,6 +7264,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="13" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -7421,13 +7425,13 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45962.842483333334" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="455" xr:uid="{8670B9A0-D18C-48F4-9D62-CC165A896835}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="David Barron" refreshedDate="45966.877235879627" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="457" xr:uid="{8670B9A0-D18C-48F4-9D62-CC165A896835}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:I750" sheet="Current account"/>
   </cacheSource>
   <cacheFields count="9">
     <cacheField name="Date" numFmtId="0">
-      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-11-02T00:00:00"/>
+      <sharedItems containsNonDate="0" containsDate="1" containsString="0" containsBlank="1" minDate="2025-01-01T00:00:00" maxDate="2025-11-05T00:00:00"/>
     </cacheField>
     <cacheField name="Type" numFmtId="0">
       <sharedItems containsBlank="1"/>
@@ -12502,7 +12506,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="455">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="457">
   <r>
     <d v="2025-01-01T00:00:00"/>
     <m/>
@@ -17498,6 +17502,28 @@
     <s v="Invoice 1027617, poster encapsulation"/>
   </r>
   <r>
+    <d v="2025-11-03T00:00:00"/>
+    <s v="SO"/>
+    <s v="JEREMY MORGAN OAS"/>
+    <n v="240"/>
+    <m/>
+    <n v="9009.1100000000024"/>
+    <x v="8"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <d v="2025-11-04T00:00:00"/>
+    <s v="BP"/>
+    <s v="Sarah Dearling OAS"/>
+    <n v="15.59"/>
+    <m/>
+    <n v="8993.5200000000023"/>
+    <x v="11"/>
+    <m/>
+    <s v="Domain name"/>
+  </r>
+  <r>
     <m/>
     <m/>
     <m/>
@@ -17512,7 +17538,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A161C15E-4B91-405B-9C74-C155CFC49E46}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A161C15E-4B91-405B-9C74-C155CFC49E46}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C32" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -17677,7 +17703,140 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A22:C35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="9">
+    <pivotField numFmtId="15" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField numFmtId="164" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="34">
+        <item x="21"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="6"/>
+        <item x="20"/>
+        <item x="9"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item m="1" x="30"/>
+        <item x="14"/>
+        <item x="3"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="13"/>
+        <item m="1" x="29"/>
+        <item x="11"/>
+        <item x="23"/>
+        <item x="0"/>
+        <item x="12"/>
+        <item x="4"/>
+        <item m="1" x="32"/>
+        <item x="5"/>
+        <item x="15"/>
+        <item m="1" x="31"/>
+        <item x="22"/>
+        <item x="1"/>
+        <item x="8"/>
+        <item x="10"/>
+        <item m="1" x="28"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="13">
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="7" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{88CC6FF2-D2D5-4EC7-9086-AAE36B3B0E13}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C17" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField numFmtId="15" showAll="0"/>
@@ -17795,139 +17954,6 @@
   </colItems>
   <pageFields count="1">
     <pageField fld="7" item="0" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Expenditure" fld="3" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2FE7C9AF-75EF-4873-8F1B-0F70A39EEC38}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A22:C35" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="9">
-    <pivotField numFmtId="15" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField numFmtId="164" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="34">
-        <item x="21"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="6"/>
-        <item x="20"/>
-        <item x="9"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item m="1" x="30"/>
-        <item x="14"/>
-        <item x="3"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="13"/>
-        <item m="1" x="29"/>
-        <item x="11"/>
-        <item x="23"/>
-        <item x="0"/>
-        <item x="12"/>
-        <item x="4"/>
-        <item m="1" x="32"/>
-        <item x="5"/>
-        <item x="15"/>
-        <item m="1" x="31"/>
-        <item x="22"/>
-        <item x="1"/>
-        <item x="8"/>
-        <item x="10"/>
-        <item m="1" x="28"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="6"/>
-  </rowFields>
-  <rowItems count="13">
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="7" item="1" hier="-1"/>
   </pageFields>
   <dataFields count="2">
     <dataField name="Sum of Income" fld="4" baseField="0" baseItem="0"/>
@@ -42700,10 +42726,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5956F534-76F9-4C2C-AE0C-5DBCF3D7B234}">
-  <dimension ref="A1:I455"/>
+  <dimension ref="A1:I457"/>
   <sheetViews>
-    <sheetView topLeftCell="A422" workbookViewId="0">
-      <selection activeCell="I456" sqref="I456"/>
+    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
+      <selection activeCell="G457" sqref="G457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -51679,7 +51705,7 @@
         <v>20</v>
       </c>
       <c r="F402" s="24">
-        <f t="shared" ref="F402:F455" si="7">F401+E402-D402</f>
+        <f t="shared" ref="F402:F457" si="7">F401+E402-D402</f>
         <v>14557.980000000003</v>
       </c>
       <c r="G402" t="s">
@@ -52965,6 +52991,51 @@
       </c>
       <c r="I455" t="s">
         <v>2320</v>
+      </c>
+    </row>
+    <row r="456" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A456" s="23">
+        <v>45964</v>
+      </c>
+      <c r="B456" t="s">
+        <v>1664</v>
+      </c>
+      <c r="C456" t="s">
+        <v>1780</v>
+      </c>
+      <c r="D456">
+        <v>240</v>
+      </c>
+      <c r="F456" s="24">
+        <f t="shared" si="7"/>
+        <v>9009.1100000000024</v>
+      </c>
+      <c r="G456" t="s">
+        <v>981</v>
+      </c>
+    </row>
+    <row r="457" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A457" s="23">
+        <v>45965</v>
+      </c>
+      <c r="B457" t="s">
+        <v>262</v>
+      </c>
+      <c r="C457" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D457">
+        <v>15.59</v>
+      </c>
+      <c r="F457" s="24">
+        <f t="shared" si="7"/>
+        <v>8993.5200000000023</v>
+      </c>
+      <c r="G457" t="s">
+        <v>7</v>
+      </c>
+      <c r="I457" t="s">
+        <v>2321</v>
       </c>
     </row>
   </sheetData>
@@ -59184,7 +59255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12A8BED0-6F25-4951-9707-565F124E30A4}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -59700,20 +59771,24 @@
       <c r="A4" s="26" t="s">
         <v>178</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="48">
         <v>6648.8800000000019</v>
       </c>
+      <c r="C4" s="48"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="26" t="s">
         <v>84</v>
       </c>
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="48"/>
+      <c r="C6" s="48">
         <v>1105</v>
       </c>
     </row>
@@ -59721,7 +59796,8 @@
       <c r="A7" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="48"/>
+      <c r="C7" s="48">
         <v>779.79</v>
       </c>
     </row>
@@ -59729,7 +59805,8 @@
       <c r="A8" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="48"/>
+      <c r="C8" s="48">
         <v>444.82000000000005</v>
       </c>
     </row>
@@ -59737,15 +59814,17 @@
       <c r="A9" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="48">
         <v>230</v>
       </c>
+      <c r="C9" s="48"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="48"/>
+      <c r="C10" s="48">
         <v>200</v>
       </c>
     </row>
@@ -59753,7 +59832,8 @@
       <c r="A11" s="26" t="s">
         <v>100</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="48"/>
+      <c r="C11" s="48">
         <v>132</v>
       </c>
     </row>
@@ -59761,15 +59841,17 @@
       <c r="A12" s="26" t="s">
         <v>981</v>
       </c>
-      <c r="C12">
-        <v>1170</v>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48">
+        <v>1410</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="48"/>
+      <c r="C13" s="48">
         <v>127.53999999999999</v>
       </c>
     </row>
@@ -59777,7 +59859,8 @@
       <c r="A14" s="26" t="s">
         <v>988</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="48"/>
+      <c r="C14" s="48">
         <v>812.5</v>
       </c>
     </row>
@@ -59785,31 +59868,35 @@
       <c r="A15" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C15">
-        <v>1881.03</v>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48">
+        <v>1896.62</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="48">
         <v>852.75</v>
       </c>
+      <c r="C16" s="48"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="48">
         <v>10129.92</v>
       </c>
+      <c r="C17" s="48"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C18">
+      <c r="B18" s="48"/>
+      <c r="C18" s="48">
         <v>1161.68</v>
       </c>
     </row>
@@ -59817,10 +59904,10 @@
       <c r="A19" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="48">
         <v>590.42000000000007</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="48">
         <v>502.44</v>
       </c>
     </row>
@@ -59828,7 +59915,8 @@
       <c r="A20" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C20">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48">
         <v>800</v>
       </c>
     </row>
@@ -59836,7 +59924,8 @@
       <c r="A21" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="C21">
+      <c r="B21" s="48"/>
+      <c r="C21" s="48">
         <v>613.22</v>
       </c>
     </row>
@@ -59844,10 +59933,10 @@
       <c r="A22" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="48">
         <v>18820.420000000002</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="48">
         <v>20</v>
       </c>
     </row>
@@ -59855,7 +59944,8 @@
       <c r="A23" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="C23">
+      <c r="B23" s="48"/>
+      <c r="C23" s="48">
         <v>13911.75</v>
       </c>
     </row>
@@ -59863,7 +59953,8 @@
       <c r="A24" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="C24">
+      <c r="B24" s="48"/>
+      <c r="C24" s="48">
         <v>3498.9</v>
       </c>
     </row>
@@ -59871,7 +59962,8 @@
       <c r="A25" s="26" t="s">
         <v>168</v>
       </c>
-      <c r="C25">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48">
         <v>1500</v>
       </c>
     </row>
@@ -59879,10 +59971,10 @@
       <c r="A26" s="26" t="s">
         <v>102</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="48">
         <v>200</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="48">
         <v>2140</v>
       </c>
     </row>
@@ -59890,7 +59982,8 @@
       <c r="A27" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="48"/>
+      <c r="C27" s="48">
         <v>303.10000000000002</v>
       </c>
     </row>
@@ -59898,7 +59991,8 @@
       <c r="A28" s="26" t="s">
         <v>1774</v>
       </c>
-      <c r="C28">
+      <c r="B28" s="48"/>
+      <c r="C28" s="48">
         <v>2296</v>
       </c>
     </row>
@@ -59906,7 +60000,8 @@
       <c r="A29" s="26" t="s">
         <v>1775</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="48"/>
+      <c r="C29" s="48">
         <v>192.5</v>
       </c>
     </row>
@@ -59914,7 +60009,8 @@
       <c r="A30" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="48"/>
+      <c r="C30" s="48">
         <v>219.54000000000002</v>
       </c>
     </row>
@@ -59922,7 +60018,8 @@
       <c r="A31" s="26" t="s">
         <v>2280</v>
       </c>
-      <c r="C31">
+      <c r="B31" s="48"/>
+      <c r="C31" s="48">
         <v>235.35</v>
       </c>
     </row>
@@ -59930,11 +60027,11 @@
       <c r="A32" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="48">
         <v>37472.39</v>
       </c>
-      <c r="C32">
-        <v>34047.159999999996</v>
+      <c r="C32" s="48">
+        <v>34302.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>